<commit_message>
some changes in ecell and in ui
</commit_message>
<xml_diff>
--- a/FrontEnd/test.xlsx
+++ b/FrontEnd/test.xlsx
@@ -338,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -369,10 +369,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -809,11 +810,15 @@
           <t xml:space="preserve">SI. No.: </t>
         </is>
       </c>
-      <c r="I5" s="8" t="inlineStr"/>
+      <c r="I5" s="8" t="inlineStr">
+        <is>
+          <t>gj</t>
+        </is>
+      </c>
       <c r="J5" s="6" t="n"/>
       <c r="K5" s="7" t="inlineStr">
         <is>
-          <t>Date: 28-Feb-22 - (Monday)</t>
+          <t>Date: 02-Mar-22 - (Wednesday)</t>
         </is>
       </c>
       <c r="L5" s="6" t="n"/>
@@ -826,7 +831,11 @@
           <t xml:space="preserve">Name: </t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr"/>
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
       <c r="F6" s="12" t="inlineStr">
         <is>
           <t>Mobile No.</t>
@@ -834,7 +843,7 @@
       </c>
       <c r="G6" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  </t>
+          <t xml:space="preserve">  gfhgg</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
@@ -842,13 +851,21 @@
           <t>Addhar No.</t>
         </is>
       </c>
-      <c r="J6" s="11" t="inlineStr"/>
+      <c r="J6" s="11" t="inlineStr">
+        <is>
+          <t>gjh</t>
+        </is>
+      </c>
       <c r="M6" s="2" t="inlineStr">
         <is>
           <t>Bill No.</t>
         </is>
       </c>
-      <c r="N6" s="14" t="inlineStr"/>
+      <c r="N6" s="14" t="inlineStr">
+        <is>
+          <t>gj</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="15" t="n"/>
@@ -949,106 +966,160 @@
       <c r="N9" s="18" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="30" t="n"/>
-      <c r="B10" s="31" t="n"/>
-      <c r="F10" s="32" t="inlineStr">
+      <c r="A10" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="31" t="inlineStr">
+        <is>
+          <t>hg</t>
+        </is>
+      </c>
+      <c r="F10" s="31" t="inlineStr">
         <is>
           <t>7113</t>
         </is>
       </c>
-      <c r="G10" s="31" t="n"/>
-      <c r="H10" s="31" t="n"/>
-      <c r="I10" s="31" t="n"/>
-      <c r="K10" s="31" t="n"/>
-      <c r="M10" s="31" t="n"/>
-      <c r="N10" s="33" t="n"/>
+      <c r="G10" s="31" t="inlineStr">
+        <is>
+          <t>jhg</t>
+        </is>
+      </c>
+      <c r="H10" s="31" t="inlineStr">
+        <is>
+          <t>jh</t>
+        </is>
+      </c>
+      <c r="I10" s="31" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="K10" s="31" t="inlineStr">
+        <is>
+          <t>jhg</t>
+        </is>
+      </c>
+      <c r="M10" s="31" t="inlineStr">
+        <is>
+          <t>gjh</t>
+        </is>
+      </c>
+      <c r="N10" s="32" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="30" t="n"/>
-      <c r="B11" s="31" t="n"/>
-      <c r="F11" s="31" t="n"/>
-      <c r="G11" s="31" t="n"/>
-      <c r="H11" s="31" t="n"/>
-      <c r="I11" s="31" t="n"/>
-      <c r="K11" s="31" t="n"/>
-      <c r="M11" s="31" t="n"/>
-      <c r="N11" s="33" t="n"/>
+      <c r="A11" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="31" t="inlineStr">
+        <is>
+          <t>gjh</t>
+        </is>
+      </c>
+      <c r="F11" s="33" t="n"/>
+      <c r="G11" s="31" t="inlineStr">
+        <is>
+          <t>hg</t>
+        </is>
+      </c>
+      <c r="H11" s="31" t="inlineStr">
+        <is>
+          <t>jhg</t>
+        </is>
+      </c>
+      <c r="I11" s="31" t="inlineStr">
+        <is>
+          <t>jhg</t>
+        </is>
+      </c>
+      <c r="K11" s="31" t="inlineStr">
+        <is>
+          <t>jh</t>
+        </is>
+      </c>
+      <c r="M11" s="31" t="inlineStr"/>
+      <c r="N11" s="32" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="30" t="n"/>
-      <c r="B12" s="31" t="n"/>
-      <c r="F12" s="31" t="n"/>
-      <c r="G12" s="31" t="n"/>
-      <c r="H12" s="31" t="n"/>
-      <c r="I12" s="31" t="n"/>
-      <c r="K12" s="31" t="n"/>
-      <c r="M12" s="31" t="n"/>
-      <c r="N12" s="33" t="n"/>
+      <c r="A12" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="B12" s="31" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="F12" s="33" t="n"/>
+      <c r="G12" s="31" t="inlineStr"/>
+      <c r="H12" s="31" t="inlineStr"/>
+      <c r="I12" s="31" t="inlineStr"/>
+      <c r="K12" s="31" t="inlineStr"/>
+      <c r="M12" s="31" t="inlineStr"/>
+      <c r="N12" s="32" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="30" t="n"/>
-      <c r="B13" s="31" t="n"/>
-      <c r="F13" s="31" t="n"/>
-      <c r="G13" s="31" t="n"/>
-      <c r="H13" s="31" t="n"/>
-      <c r="I13" s="31" t="n"/>
-      <c r="K13" s="31" t="n"/>
-      <c r="M13" s="31" t="n"/>
-      <c r="N13" s="33" t="n"/>
+      <c r="A13" s="34" t="n"/>
+      <c r="B13" s="33" t="n"/>
+      <c r="F13" s="33" t="n"/>
+      <c r="G13" s="33" t="n"/>
+      <c r="H13" s="33" t="n"/>
+      <c r="I13" s="33" t="n"/>
+      <c r="K13" s="33" t="n"/>
+      <c r="M13" s="33" t="n"/>
+      <c r="N13" s="32" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="30" t="n"/>
-      <c r="B14" s="31" t="n"/>
-      <c r="F14" s="31" t="n"/>
-      <c r="G14" s="31" t="n"/>
-      <c r="H14" s="31" t="n"/>
-      <c r="I14" s="31" t="n"/>
-      <c r="K14" s="31" t="n"/>
-      <c r="M14" s="31" t="n"/>
-      <c r="N14" s="33" t="n"/>
+      <c r="A14" s="34" t="n"/>
+      <c r="B14" s="33" t="n"/>
+      <c r="F14" s="33" t="n"/>
+      <c r="G14" s="33" t="n"/>
+      <c r="H14" s="33" t="n"/>
+      <c r="I14" s="33" t="n"/>
+      <c r="K14" s="33" t="n"/>
+      <c r="M14" s="33" t="n"/>
+      <c r="N14" s="32" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="30" t="n"/>
-      <c r="B15" s="31" t="n"/>
-      <c r="F15" s="31" t="n"/>
-      <c r="G15" s="31" t="n"/>
-      <c r="H15" s="31" t="n"/>
-      <c r="I15" s="31" t="n"/>
-      <c r="K15" s="31" t="n"/>
-      <c r="M15" s="31" t="n"/>
-      <c r="N15" s="33" t="n"/>
+      <c r="A15" s="34" t="n"/>
+      <c r="B15" s="33" t="n"/>
+      <c r="F15" s="33" t="n"/>
+      <c r="G15" s="33" t="n"/>
+      <c r="H15" s="33" t="n"/>
+      <c r="I15" s="33" t="n"/>
+      <c r="K15" s="33" t="n"/>
+      <c r="M15" s="33" t="n"/>
+      <c r="N15" s="32" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="30" t="n"/>
-      <c r="B16" s="31" t="n"/>
-      <c r="F16" s="31" t="n"/>
-      <c r="G16" s="31" t="n"/>
-      <c r="H16" s="31" t="n"/>
-      <c r="I16" s="31" t="n"/>
-      <c r="K16" s="31" t="n"/>
-      <c r="M16" s="31" t="n"/>
-      <c r="N16" s="33" t="n"/>
+      <c r="A16" s="34" t="n"/>
+      <c r="B16" s="33" t="n"/>
+      <c r="F16" s="33" t="n"/>
+      <c r="G16" s="33" t="n"/>
+      <c r="H16" s="33" t="n"/>
+      <c r="I16" s="33" t="n"/>
+      <c r="K16" s="33" t="n"/>
+      <c r="M16" s="33" t="n"/>
+      <c r="N16" s="32" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="30" t="n"/>
-      <c r="B17" s="31" t="n"/>
-      <c r="F17" s="31" t="n"/>
-      <c r="G17" s="31" t="n"/>
-      <c r="H17" s="31" t="n"/>
-      <c r="I17" s="31" t="n"/>
-      <c r="K17" s="31" t="n"/>
-      <c r="M17" s="31" t="n"/>
-      <c r="N17" s="33" t="n"/>
+      <c r="A17" s="34" t="n"/>
+      <c r="B17" s="33" t="n"/>
+      <c r="F17" s="33" t="n"/>
+      <c r="G17" s="33" t="n"/>
+      <c r="H17" s="33" t="n"/>
+      <c r="I17" s="33" t="n"/>
+      <c r="K17" s="33" t="n"/>
+      <c r="M17" s="33" t="n"/>
+      <c r="N17" s="32" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="34" t="n"/>
+      <c r="A18" s="35" t="n"/>
       <c r="B18" s="25" t="n"/>
       <c r="C18" s="26" t="n"/>
       <c r="D18" s="26" t="n"/>
       <c r="E18" s="27" t="n"/>
-      <c r="F18" s="35" t="n"/>
-      <c r="G18" s="35" t="n"/>
-      <c r="H18" s="35" t="n"/>
+      <c r="F18" s="36" t="n"/>
+      <c r="G18" s="36" t="n"/>
+      <c r="H18" s="36" t="n"/>
       <c r="I18" s="25" t="n"/>
       <c r="J18" s="27" t="n"/>
       <c r="K18" s="25" t="n"/>
@@ -1057,25 +1128,25 @@
       <c r="N18" s="18" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="36" t="n"/>
-      <c r="D19" s="37" t="inlineStr">
+      <c r="A19" s="37" t="n"/>
+      <c r="D19" s="38" t="inlineStr">
         <is>
           <t>Old Jewellery</t>
         </is>
       </c>
-      <c r="H19" s="38" t="n"/>
-      <c r="I19" s="39" t="inlineStr">
+      <c r="H19" s="39" t="n"/>
+      <c r="I19" s="40" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="J19" s="40" t="inlineStr">
+      <c r="J19" s="41" t="inlineStr">
         <is>
           <t>Unit Price</t>
         </is>
       </c>
-      <c r="L19" s="38" t="n"/>
-      <c r="M19" s="39" t="inlineStr">
+      <c r="L19" s="39" t="n"/>
+      <c r="M19" s="40" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -1083,62 +1154,169 @@
       <c r="N19" s="24" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="30" t="n"/>
-      <c r="H20" s="31" t="n"/>
-      <c r="J20" s="31" t="n"/>
-      <c r="L20" s="31" t="n"/>
-      <c r="N20" s="33" t="n"/>
+      <c r="A20" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="42" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="H20" s="33" t="n"/>
+      <c r="I20" s="42" t="inlineStr">
+        <is>
+          <t>hjh</t>
+        </is>
+      </c>
+      <c r="J20" s="31" t="inlineStr">
+        <is>
+          <t>jh</t>
+        </is>
+      </c>
+      <c r="L20" s="33" t="n"/>
+      <c r="M20" s="42" t="inlineStr">
+        <is>
+          <t>gjh</t>
+        </is>
+      </c>
+      <c r="N20" s="32" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="30" t="n"/>
-      <c r="H21" s="31" t="n"/>
-      <c r="I21" s="41" t="inlineStr"/>
-      <c r="J21" s="32" t="inlineStr"/>
-      <c r="L21" s="31" t="n"/>
-      <c r="M21" s="41" t="inlineStr"/>
-      <c r="N21" s="33" t="n"/>
+      <c r="A21" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="B21" s="42" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="H21" s="33" t="n"/>
+      <c r="I21" s="42" t="inlineStr">
+        <is>
+          <t>jhg</t>
+        </is>
+      </c>
+      <c r="J21" s="31" t="inlineStr">
+        <is>
+          <t>jh</t>
+        </is>
+      </c>
+      <c r="L21" s="33" t="n"/>
+      <c r="M21" s="42" t="inlineStr">
+        <is>
+          <t>gjh</t>
+        </is>
+      </c>
+      <c r="N21" s="32" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="30" t="n"/>
-      <c r="H22" s="31" t="n"/>
-      <c r="J22" s="31" t="n"/>
-      <c r="L22" s="31" t="n"/>
-      <c r="N22" s="33" t="n"/>
+      <c r="A22" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="B22" s="42" t="inlineStr">
+        <is>
+          <t>gj</t>
+        </is>
+      </c>
+      <c r="H22" s="33" t="n"/>
+      <c r="I22" s="42" t="inlineStr">
+        <is>
+          <t>hg</t>
+        </is>
+      </c>
+      <c r="J22" s="31" t="inlineStr">
+        <is>
+          <t>jhg</t>
+        </is>
+      </c>
+      <c r="L22" s="33" t="n"/>
+      <c r="M22" s="42" t="inlineStr">
+        <is>
+          <t>jhg</t>
+        </is>
+      </c>
+      <c r="N22" s="32" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="30" t="n"/>
-      <c r="H23" s="31" t="n"/>
-      <c r="J23" s="31" t="n"/>
-      <c r="L23" s="31" t="n"/>
-      <c r="N23" s="33" t="n"/>
+      <c r="A23" s="34" t="n"/>
+      <c r="H23" s="33" t="n"/>
+      <c r="J23" s="33" t="n"/>
+      <c r="L23" s="33" t="n"/>
+      <c r="N23" s="32" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="30" t="n"/>
-      <c r="H24" s="31" t="n"/>
-      <c r="J24" s="31" t="n"/>
-      <c r="L24" s="31" t="n"/>
-      <c r="N24" s="33" t="n"/>
+      <c r="A24" s="34" t="n"/>
+      <c r="D24" s="40" t="inlineStr">
+        <is>
+          <t>Other Addition Or Deduction</t>
+        </is>
+      </c>
+      <c r="H24" s="33" t="n"/>
+      <c r="J24" s="33" t="n"/>
+      <c r="L24" s="33" t="n"/>
+      <c r="M24" s="40" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="N24" s="32" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="30" t="n"/>
-      <c r="H25" s="31" t="n"/>
-      <c r="J25" s="31" t="n"/>
-      <c r="L25" s="31" t="n"/>
-      <c r="N25" s="33" t="n"/>
+      <c r="A25" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" s="42" t="inlineStr">
+        <is>
+          <t>bhkj</t>
+        </is>
+      </c>
+      <c r="H25" s="33" t="n"/>
+      <c r="J25" s="33" t="n"/>
+      <c r="L25" s="33" t="n"/>
+      <c r="M25" s="42" t="inlineStr">
+        <is>
+          <t>hj</t>
+        </is>
+      </c>
+      <c r="N25" s="32" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="30" t="n"/>
-      <c r="H26" s="31" t="n"/>
-      <c r="J26" s="31" t="n"/>
-      <c r="L26" s="31" t="n"/>
-      <c r="N26" s="33" t="n"/>
+      <c r="A26" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" s="42" t="inlineStr">
+        <is>
+          <t>jk</t>
+        </is>
+      </c>
+      <c r="H26" s="33" t="n"/>
+      <c r="J26" s="33" t="n"/>
+      <c r="L26" s="33" t="n"/>
+      <c r="M26" s="42" t="inlineStr">
+        <is>
+          <t>hkj</t>
+        </is>
+      </c>
+      <c r="N26" s="32" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="30" t="n"/>
-      <c r="H27" s="31" t="n"/>
-      <c r="J27" s="31" t="n"/>
-      <c r="L27" s="31" t="n"/>
-      <c r="N27" s="33" t="n"/>
+      <c r="A27" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="D27" s="42" t="inlineStr">
+        <is>
+          <t>hkj</t>
+        </is>
+      </c>
+      <c r="H27" s="33" t="n"/>
+      <c r="J27" s="33" t="n"/>
+      <c r="L27" s="33" t="n"/>
+      <c r="M27" s="42" t="inlineStr">
+        <is>
+          <t>h</t>
+        </is>
+      </c>
+      <c r="N27" s="32" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="15" t="n"/>
@@ -1148,121 +1326,121 @@
       <c r="N28" s="18" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="42" t="n"/>
-      <c r="B29" s="43" t="n"/>
-      <c r="C29" s="43" t="n"/>
-      <c r="D29" s="43" t="n"/>
-      <c r="E29" s="44" t="inlineStr">
+      <c r="A29" s="43" t="n"/>
+      <c r="B29" s="44" t="n"/>
+      <c r="C29" s="44" t="n"/>
+      <c r="D29" s="44" t="n"/>
+      <c r="E29" s="45" t="inlineStr">
         <is>
           <t>Mode Of Payment</t>
         </is>
       </c>
-      <c r="F29" s="43" t="n"/>
-      <c r="G29" s="43" t="n"/>
-      <c r="H29" s="43" t="n"/>
-      <c r="I29" s="45" t="inlineStr">
+      <c r="F29" s="44" t="n"/>
+      <c r="G29" s="44" t="n"/>
+      <c r="H29" s="44" t="n"/>
+      <c r="I29" s="46" t="inlineStr">
         <is>
           <t>Cash</t>
         </is>
       </c>
-      <c r="J29" s="43" t="n"/>
-      <c r="K29" s="43" t="n"/>
-      <c r="L29" s="43" t="n"/>
-      <c r="M29" s="43" t="n"/>
-      <c r="N29" s="46" t="n"/>
+      <c r="J29" s="44" t="n"/>
+      <c r="K29" s="44" t="n"/>
+      <c r="L29" s="44" t="n"/>
+      <c r="M29" s="44" t="n"/>
+      <c r="N29" s="47" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="47" t="inlineStr">
+      <c r="A30" s="48" t="inlineStr">
         <is>
           <t>Total in Words</t>
         </is>
       </c>
-      <c r="B30" s="43" t="n"/>
-      <c r="C30" s="45" t="inlineStr">
+      <c r="B30" s="44" t="n"/>
+      <c r="C30" s="46" t="inlineStr">
         <is>
           <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
         </is>
       </c>
-      <c r="D30" s="43" t="n"/>
-      <c r="E30" s="43" t="n"/>
-      <c r="F30" s="43" t="n"/>
-      <c r="G30" s="43" t="n"/>
-      <c r="H30" s="43" t="n"/>
-      <c r="I30" s="43" t="n"/>
-      <c r="J30" s="48" t="inlineStr">
+      <c r="D30" s="44" t="n"/>
+      <c r="E30" s="44" t="n"/>
+      <c r="F30" s="44" t="n"/>
+      <c r="G30" s="44" t="n"/>
+      <c r="H30" s="44" t="n"/>
+      <c r="I30" s="44" t="n"/>
+      <c r="J30" s="49" t="inlineStr">
         <is>
           <t xml:space="preserve">Total Paid : </t>
         </is>
       </c>
-      <c r="K30" s="43" t="n"/>
-      <c r="L30" s="45" t="inlineStr">
+      <c r="K30" s="44" t="n"/>
+      <c r="L30" s="46" t="inlineStr">
         <is>
           <t>2000000</t>
         </is>
       </c>
-      <c r="M30" s="43" t="n"/>
-      <c r="N30" s="46" t="n"/>
+      <c r="M30" s="44" t="n"/>
+      <c r="N30" s="47" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="36" t="n"/>
-      <c r="B31" s="37" t="inlineStr">
+      <c r="A31" s="37" t="n"/>
+      <c r="B31" s="38" t="inlineStr">
         <is>
           <t>Terms and conditions</t>
         </is>
       </c>
-      <c r="J31" s="38" t="n"/>
-      <c r="N31" s="33" t="n"/>
+      <c r="J31" s="39" t="n"/>
+      <c r="N31" s="32" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="49" t="inlineStr">
+      <c r="A32" s="50" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. Before taking delivery Customer should check the ornaments by piece and weight. </t>
         </is>
       </c>
-      <c r="J32" s="31" t="n"/>
-      <c r="N32" s="33" t="n"/>
+      <c r="J32" s="33" t="n"/>
+      <c r="N32" s="32" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="49" t="inlineStr">
+      <c r="A33" s="50" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2. Exchange your ornaments within 7 days in good condition.</t>
         </is>
       </c>
-      <c r="J33" s="31" t="n"/>
-      <c r="N33" s="33" t="n"/>
+      <c r="J33" s="33" t="n"/>
+      <c r="N33" s="32" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="49" t="inlineStr">
+      <c r="A34" s="50" t="inlineStr">
         <is>
           <t xml:space="preserve"> 3. We are not responsible for any damage or brakage after delivery</t>
         </is>
       </c>
-      <c r="J34" s="31" t="n"/>
-      <c r="N34" s="33" t="n"/>
+      <c r="J34" s="33" t="n"/>
+      <c r="N34" s="32" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="49" t="inlineStr">
+      <c r="A35" s="50" t="inlineStr">
         <is>
           <t xml:space="preserve"> 4. We can repair the ornaments if possible</t>
         </is>
       </c>
-      <c r="J35" s="31" t="n"/>
-      <c r="N35" s="50" t="n"/>
+      <c r="J35" s="33" t="n"/>
+      <c r="N35" s="51" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="51" t="n"/>
-      <c r="B36" s="51" t="n"/>
-      <c r="C36" s="51" t="n"/>
-      <c r="D36" s="51" t="n"/>
-      <c r="E36" s="51" t="n"/>
-      <c r="F36" s="51" t="n"/>
-      <c r="G36" s="51" t="n"/>
-      <c r="H36" s="51" t="n"/>
-      <c r="I36" s="51" t="n"/>
-      <c r="J36" s="51" t="n"/>
-      <c r="K36" s="51" t="n"/>
-      <c r="L36" s="51" t="n"/>
-      <c r="M36" s="51" t="n"/>
+      <c r="A36" s="52" t="n"/>
+      <c r="B36" s="52" t="n"/>
+      <c r="C36" s="52" t="n"/>
+      <c r="D36" s="52" t="n"/>
+      <c r="E36" s="52" t="n"/>
+      <c r="F36" s="52" t="n"/>
+      <c r="G36" s="52" t="n"/>
+      <c r="H36" s="52" t="n"/>
+      <c r="I36" s="52" t="n"/>
+      <c r="J36" s="52" t="n"/>
+      <c r="K36" s="52" t="n"/>
+      <c r="L36" s="52" t="n"/>
+      <c r="M36" s="52" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.2" top="0.2" bottom="0.2" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Made the ui bit user friendly and added to find the cust info from cust number then calculate the cost gst and all after putting mc
</commit_message>
<xml_diff>
--- a/FrontEnd/test.xlsx
+++ b/FrontEnd/test.xlsx
@@ -369,11 +369,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -381,6 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -810,15 +810,11 @@
           <t xml:space="preserve">SI. No.: </t>
         </is>
       </c>
-      <c r="I5" s="8" t="inlineStr">
-        <is>
-          <t>232</t>
-        </is>
-      </c>
+      <c r="I5" s="8" t="inlineStr"/>
       <c r="J5" s="6" t="n"/>
       <c r="K5" s="7" t="inlineStr">
         <is>
-          <t>Date: 02-Mar-22 - (Wednesday)</t>
+          <t>Date: 03-Mar-22 - (Thursday)</t>
         </is>
       </c>
       <c r="L5" s="6" t="n"/>
@@ -831,11 +827,7 @@
           <t xml:space="preserve">Name: </t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr">
-        <is>
-          <t>dfafd</t>
-        </is>
-      </c>
+      <c r="B6" s="11" t="inlineStr"/>
       <c r="F6" s="12" t="inlineStr">
         <is>
           <t>Mobile No.</t>
@@ -843,7 +835,7 @@
       </c>
       <c r="G6" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  78931</t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
@@ -851,21 +843,13 @@
           <t>Addhar No.</t>
         </is>
       </c>
-      <c r="J6" s="11" t="inlineStr">
-        <is>
-          <t>232</t>
-        </is>
-      </c>
+      <c r="J6" s="11" t="inlineStr"/>
       <c r="M6" s="2" t="inlineStr">
         <is>
           <t>Bill No.</t>
         </is>
       </c>
-      <c r="N6" s="14" t="inlineStr">
-        <is>
-          <t>232</t>
-        </is>
-      </c>
+      <c r="N6" s="14" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="15" t="n"/>
@@ -966,132 +950,106 @@
       <c r="N9" s="18" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="31" t="inlineStr">
-        <is>
-          <t>sfsfs</t>
-        </is>
-      </c>
-      <c r="F10" s="31" t="inlineStr">
+      <c r="A10" s="30" t="n"/>
+      <c r="B10" s="31" t="n"/>
+      <c r="F10" s="32" t="inlineStr">
         <is>
           <t>7113</t>
         </is>
       </c>
-      <c r="G10" s="31" t="inlineStr">
-        <is>
-          <t>232</t>
-        </is>
-      </c>
-      <c r="H10" s="31" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="I10" s="31" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="K10" s="31" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="M10" s="31" t="inlineStr">
-        <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="N10" s="32" t="n"/>
+      <c r="G10" s="31" t="n"/>
+      <c r="H10" s="31" t="n"/>
+      <c r="I10" s="31" t="n"/>
+      <c r="K10" s="31" t="n"/>
+      <c r="M10" s="31" t="n"/>
+      <c r="N10" s="33" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="33" t="n"/>
-      <c r="B11" s="34" t="n"/>
-      <c r="F11" s="34" t="n"/>
-      <c r="G11" s="34" t="n"/>
-      <c r="H11" s="34" t="n"/>
-      <c r="I11" s="34" t="n"/>
-      <c r="K11" s="34" t="n"/>
-      <c r="M11" s="34" t="n"/>
-      <c r="N11" s="32" t="n"/>
+      <c r="A11" s="30" t="n"/>
+      <c r="B11" s="31" t="n"/>
+      <c r="F11" s="31" t="n"/>
+      <c r="G11" s="31" t="n"/>
+      <c r="H11" s="31" t="n"/>
+      <c r="I11" s="31" t="n"/>
+      <c r="K11" s="31" t="n"/>
+      <c r="M11" s="31" t="n"/>
+      <c r="N11" s="33" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="33" t="n"/>
-      <c r="B12" s="34" t="n"/>
-      <c r="F12" s="34" t="n"/>
-      <c r="G12" s="34" t="n"/>
-      <c r="H12" s="34" t="n"/>
-      <c r="I12" s="34" t="n"/>
-      <c r="K12" s="34" t="n"/>
-      <c r="M12" s="34" t="n"/>
-      <c r="N12" s="32" t="n"/>
+      <c r="A12" s="30" t="n"/>
+      <c r="B12" s="31" t="n"/>
+      <c r="F12" s="31" t="n"/>
+      <c r="G12" s="31" t="n"/>
+      <c r="H12" s="31" t="n"/>
+      <c r="I12" s="31" t="n"/>
+      <c r="K12" s="31" t="n"/>
+      <c r="M12" s="31" t="n"/>
+      <c r="N12" s="33" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="33" t="n"/>
-      <c r="B13" s="34" t="n"/>
-      <c r="F13" s="34" t="n"/>
-      <c r="G13" s="34" t="n"/>
-      <c r="H13" s="34" t="n"/>
-      <c r="I13" s="34" t="n"/>
-      <c r="K13" s="34" t="n"/>
-      <c r="M13" s="34" t="n"/>
-      <c r="N13" s="32" t="n"/>
+      <c r="A13" s="30" t="n"/>
+      <c r="B13" s="31" t="n"/>
+      <c r="F13" s="31" t="n"/>
+      <c r="G13" s="31" t="n"/>
+      <c r="H13" s="31" t="n"/>
+      <c r="I13" s="31" t="n"/>
+      <c r="K13" s="31" t="n"/>
+      <c r="M13" s="31" t="n"/>
+      <c r="N13" s="33" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="33" t="n"/>
-      <c r="B14" s="34" t="n"/>
-      <c r="F14" s="34" t="n"/>
-      <c r="G14" s="34" t="n"/>
-      <c r="H14" s="34" t="n"/>
-      <c r="I14" s="34" t="n"/>
-      <c r="K14" s="34" t="n"/>
-      <c r="M14" s="34" t="n"/>
-      <c r="N14" s="32" t="n"/>
+      <c r="A14" s="30" t="n"/>
+      <c r="B14" s="31" t="n"/>
+      <c r="F14" s="31" t="n"/>
+      <c r="G14" s="31" t="n"/>
+      <c r="H14" s="31" t="n"/>
+      <c r="I14" s="31" t="n"/>
+      <c r="K14" s="31" t="n"/>
+      <c r="M14" s="31" t="n"/>
+      <c r="N14" s="33" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="33" t="n"/>
-      <c r="B15" s="34" t="n"/>
-      <c r="F15" s="34" t="n"/>
-      <c r="G15" s="34" t="n"/>
-      <c r="H15" s="34" t="n"/>
-      <c r="I15" s="34" t="n"/>
-      <c r="K15" s="34" t="n"/>
-      <c r="M15" s="34" t="n"/>
-      <c r="N15" s="32" t="n"/>
+      <c r="A15" s="30" t="n"/>
+      <c r="B15" s="31" t="n"/>
+      <c r="F15" s="31" t="n"/>
+      <c r="G15" s="31" t="n"/>
+      <c r="H15" s="31" t="n"/>
+      <c r="I15" s="31" t="n"/>
+      <c r="K15" s="31" t="n"/>
+      <c r="M15" s="31" t="n"/>
+      <c r="N15" s="33" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="33" t="n"/>
-      <c r="B16" s="34" t="n"/>
-      <c r="F16" s="34" t="n"/>
-      <c r="G16" s="34" t="n"/>
-      <c r="H16" s="34" t="n"/>
-      <c r="I16" s="34" t="n"/>
-      <c r="K16" s="34" t="n"/>
-      <c r="M16" s="34" t="n"/>
-      <c r="N16" s="32" t="n"/>
+      <c r="A16" s="30" t="n"/>
+      <c r="B16" s="31" t="n"/>
+      <c r="F16" s="31" t="n"/>
+      <c r="G16" s="31" t="n"/>
+      <c r="H16" s="31" t="n"/>
+      <c r="I16" s="31" t="n"/>
+      <c r="K16" s="31" t="n"/>
+      <c r="M16" s="31" t="n"/>
+      <c r="N16" s="33" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="33" t="n"/>
-      <c r="B17" s="34" t="n"/>
-      <c r="F17" s="34" t="n"/>
-      <c r="G17" s="34" t="n"/>
-      <c r="H17" s="34" t="n"/>
-      <c r="I17" s="34" t="n"/>
-      <c r="K17" s="34" t="n"/>
-      <c r="M17" s="34" t="n"/>
-      <c r="N17" s="32" t="n"/>
+      <c r="A17" s="30" t="n"/>
+      <c r="B17" s="31" t="n"/>
+      <c r="F17" s="31" t="n"/>
+      <c r="G17" s="31" t="n"/>
+      <c r="H17" s="31" t="n"/>
+      <c r="I17" s="31" t="n"/>
+      <c r="K17" s="31" t="n"/>
+      <c r="M17" s="31" t="n"/>
+      <c r="N17" s="33" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="35" t="n"/>
+      <c r="A18" s="34" t="n"/>
       <c r="B18" s="25" t="n"/>
       <c r="C18" s="26" t="n"/>
       <c r="D18" s="26" t="n"/>
       <c r="E18" s="27" t="n"/>
-      <c r="F18" s="36" t="n"/>
-      <c r="G18" s="36" t="n"/>
-      <c r="H18" s="36" t="n"/>
+      <c r="F18" s="35" t="n"/>
+      <c r="G18" s="35" t="n"/>
+      <c r="H18" s="35" t="n"/>
       <c r="I18" s="25" t="n"/>
       <c r="J18" s="27" t="n"/>
       <c r="K18" s="25" t="n"/>
@@ -1100,25 +1058,25 @@
       <c r="N18" s="18" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="37" t="n"/>
-      <c r="D19" s="38" t="inlineStr">
+      <c r="A19" s="36" t="n"/>
+      <c r="D19" s="37" t="inlineStr">
         <is>
           <t>Old Jewellery</t>
         </is>
       </c>
-      <c r="H19" s="39" t="n"/>
-      <c r="I19" s="40" t="inlineStr">
+      <c r="H19" s="38" t="n"/>
+      <c r="I19" s="39" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="J19" s="41" t="inlineStr">
+      <c r="J19" s="40" t="inlineStr">
         <is>
           <t>Unit Price</t>
         </is>
       </c>
-      <c r="L19" s="39" t="n"/>
-      <c r="M19" s="40" t="inlineStr">
+      <c r="L19" s="38" t="n"/>
+      <c r="M19" s="39" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -1126,85 +1084,85 @@
       <c r="N19" s="24" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="30" t="n">
+      <c r="A20" s="41" t="n">
         <v>1</v>
       </c>
       <c r="B20" s="42" t="inlineStr"/>
-      <c r="H20" s="34" t="n"/>
+      <c r="H20" s="31" t="n"/>
       <c r="I20" s="42" t="inlineStr"/>
-      <c r="J20" s="31" t="inlineStr"/>
-      <c r="L20" s="34" t="n"/>
+      <c r="J20" s="32" t="inlineStr"/>
+      <c r="L20" s="31" t="n"/>
       <c r="M20" s="42" t="inlineStr"/>
-      <c r="N20" s="32" t="n"/>
+      <c r="N20" s="33" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="30" t="n">
+      <c r="A21" s="41" t="n">
         <v>2</v>
       </c>
       <c r="B21" s="42" t="inlineStr"/>
-      <c r="H21" s="34" t="n"/>
+      <c r="H21" s="31" t="n"/>
       <c r="I21" s="42" t="inlineStr"/>
-      <c r="J21" s="31" t="inlineStr"/>
-      <c r="L21" s="34" t="n"/>
+      <c r="J21" s="32" t="inlineStr"/>
+      <c r="L21" s="31" t="n"/>
       <c r="M21" s="42" t="inlineStr"/>
-      <c r="N21" s="32" t="n"/>
+      <c r="N21" s="33" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="30" t="n">
+      <c r="A22" s="41" t="n">
         <v>3</v>
       </c>
       <c r="B22" s="42" t="inlineStr"/>
-      <c r="H22" s="34" t="n"/>
+      <c r="H22" s="31" t="n"/>
       <c r="I22" s="42" t="inlineStr"/>
-      <c r="J22" s="31" t="inlineStr"/>
-      <c r="L22" s="34" t="n"/>
+      <c r="J22" s="32" t="inlineStr"/>
+      <c r="L22" s="31" t="n"/>
       <c r="M22" s="42" t="inlineStr"/>
-      <c r="N22" s="32" t="n"/>
+      <c r="N22" s="33" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="33" t="n"/>
-      <c r="H23" s="34" t="n"/>
-      <c r="J23" s="34" t="n"/>
-      <c r="L23" s="34" t="n"/>
-      <c r="N23" s="32" t="n"/>
+      <c r="A23" s="30" t="n"/>
+      <c r="H23" s="31" t="n"/>
+      <c r="J23" s="31" t="n"/>
+      <c r="L23" s="31" t="n"/>
+      <c r="N23" s="33" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="33" t="n"/>
-      <c r="D24" s="40" t="inlineStr">
+      <c r="A24" s="30" t="n"/>
+      <c r="D24" s="39" t="inlineStr">
         <is>
           <t>Other Addition Or Deduction</t>
         </is>
       </c>
-      <c r="H24" s="34" t="n"/>
-      <c r="J24" s="34" t="n"/>
-      <c r="L24" s="34" t="n"/>
-      <c r="M24" s="40" t="inlineStr">
+      <c r="H24" s="31" t="n"/>
+      <c r="J24" s="31" t="n"/>
+      <c r="L24" s="31" t="n"/>
+      <c r="M24" s="39" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="N24" s="32" t="n"/>
+      <c r="N24" s="33" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="33" t="n"/>
-      <c r="H25" s="34" t="n"/>
-      <c r="J25" s="34" t="n"/>
-      <c r="L25" s="34" t="n"/>
-      <c r="N25" s="32" t="n"/>
+      <c r="A25" s="30" t="n"/>
+      <c r="H25" s="31" t="n"/>
+      <c r="J25" s="31" t="n"/>
+      <c r="L25" s="31" t="n"/>
+      <c r="N25" s="33" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="33" t="n"/>
-      <c r="H26" s="34" t="n"/>
-      <c r="J26" s="34" t="n"/>
-      <c r="L26" s="34" t="n"/>
-      <c r="N26" s="32" t="n"/>
+      <c r="A26" s="30" t="n"/>
+      <c r="H26" s="31" t="n"/>
+      <c r="J26" s="31" t="n"/>
+      <c r="L26" s="31" t="n"/>
+      <c r="N26" s="33" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="33" t="n"/>
-      <c r="H27" s="34" t="n"/>
-      <c r="J27" s="34" t="n"/>
-      <c r="L27" s="34" t="n"/>
-      <c r="N27" s="32" t="n"/>
+      <c r="A27" s="30" t="n"/>
+      <c r="H27" s="31" t="n"/>
+      <c r="J27" s="31" t="n"/>
+      <c r="L27" s="31" t="n"/>
+      <c r="N27" s="33" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="15" t="n"/>
@@ -1270,14 +1228,14 @@
       <c r="N30" s="47" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="37" t="n"/>
-      <c r="B31" s="38" t="inlineStr">
+      <c r="A31" s="36" t="n"/>
+      <c r="B31" s="37" t="inlineStr">
         <is>
           <t>Terms and conditions</t>
         </is>
       </c>
-      <c r="J31" s="39" t="n"/>
-      <c r="N31" s="32" t="n"/>
+      <c r="J31" s="38" t="n"/>
+      <c r="N31" s="33" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="50" t="inlineStr">
@@ -1285,8 +1243,8 @@
           <t xml:space="preserve"> 1. Before taking delivery Customer should check the ornaments by piece and weight. </t>
         </is>
       </c>
-      <c r="J32" s="34" t="n"/>
-      <c r="N32" s="32" t="n"/>
+      <c r="J32" s="31" t="n"/>
+      <c r="N32" s="33" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="50" t="inlineStr">
@@ -1294,8 +1252,8 @@
           <t xml:space="preserve"> 2. Exchange your ornaments within 7 days in good condition.</t>
         </is>
       </c>
-      <c r="J33" s="34" t="n"/>
-      <c r="N33" s="32" t="n"/>
+      <c r="J33" s="31" t="n"/>
+      <c r="N33" s="33" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="50" t="inlineStr">
@@ -1303,8 +1261,8 @@
           <t xml:space="preserve"> 3. We are not responsible for any damage or brakage after delivery</t>
         </is>
       </c>
-      <c r="J34" s="34" t="n"/>
-      <c r="N34" s="32" t="n"/>
+      <c r="J34" s="31" t="n"/>
+      <c r="N34" s="33" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="50" t="inlineStr">
@@ -1312,7 +1270,7 @@
           <t xml:space="preserve"> 4. We can repair the ornaments if possible</t>
         </is>
       </c>
-      <c r="J35" s="34" t="n"/>
+      <c r="J35" s="31" t="n"/>
       <c r="N35" s="51" t="n"/>
     </row>
     <row r="36">

</xml_diff>

<commit_message>
added old gold unit price
</commit_message>
<xml_diff>
--- a/FrontEnd/test.xlsx
+++ b/FrontEnd/test.xlsx
@@ -1090,7 +1090,11 @@
       <c r="B20" s="42" t="inlineStr"/>
       <c r="H20" s="31" t="n"/>
       <c r="I20" s="42" t="inlineStr"/>
-      <c r="J20" s="32" t="inlineStr"/>
+      <c r="J20" s="32" t="inlineStr">
+        <is>
+          <t>4400</t>
+        </is>
+      </c>
       <c r="L20" s="31" t="n"/>
       <c r="M20" s="42" t="inlineStr"/>
       <c r="N20" s="33" t="n"/>
@@ -1102,7 +1106,11 @@
       <c r="B21" s="42" t="inlineStr"/>
       <c r="H21" s="31" t="n"/>
       <c r="I21" s="42" t="inlineStr"/>
-      <c r="J21" s="32" t="inlineStr"/>
+      <c r="J21" s="32" t="inlineStr">
+        <is>
+          <t>4400</t>
+        </is>
+      </c>
       <c r="L21" s="31" t="n"/>
       <c r="M21" s="42" t="inlineStr"/>
       <c r="N21" s="33" t="n"/>
@@ -1114,7 +1122,11 @@
       <c r="B22" s="42" t="inlineStr"/>
       <c r="H22" s="31" t="n"/>
       <c r="I22" s="42" t="inlineStr"/>
-      <c r="J22" s="32" t="inlineStr"/>
+      <c r="J22" s="32" t="inlineStr">
+        <is>
+          <t>4400</t>
+        </is>
+      </c>
       <c r="L22" s="31" t="n"/>
       <c r="M22" s="42" t="inlineStr"/>
       <c r="N22" s="33" t="n"/>

</xml_diff>

<commit_message>
tab tab next added to all fields
</commit_message>
<xml_diff>
--- a/FrontEnd/test.xlsx
+++ b/FrontEnd/test.xlsx
@@ -368,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -399,10 +399,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -850,7 +851,7 @@
       <c r="J5" s="6" t="n"/>
       <c r="K5" s="7" t="inlineStr">
         <is>
-          <t>Date: 03-Mar-22 - (Thursday)</t>
+          <t>Date: 04-Mar-22 - (Friday)</t>
         </is>
       </c>
       <c r="L5" s="6" t="n"/>
@@ -863,7 +864,11 @@
           <t xml:space="preserve">Name: </t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr"/>
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>ashu</t>
+        </is>
+      </c>
       <c r="F6" s="12" t="inlineStr">
         <is>
           <t>Mobile No.</t>
@@ -871,7 +876,7 @@
       </c>
       <c r="G6" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  </t>
+          <t xml:space="preserve">  7894100604</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
@@ -879,7 +884,11 @@
           <t>Addhar No.</t>
         </is>
       </c>
-      <c r="J6" s="11" t="inlineStr"/>
+      <c r="J6" s="11" t="inlineStr">
+        <is>
+          <t>old town</t>
+        </is>
+      </c>
       <c r="M6" s="2" t="inlineStr">
         <is>
           <t>Bill No.</t>
@@ -986,106 +995,132 @@
       <c r="N9" s="18" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="30" t="n"/>
-      <c r="B10" s="31" t="n"/>
-      <c r="F10" s="32" t="inlineStr">
+      <c r="A10" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="31" t="inlineStr">
+        <is>
+          <t>Ring</t>
+        </is>
+      </c>
+      <c r="F10" s="31" t="inlineStr">
         <is>
           <t>7113</t>
         </is>
       </c>
-      <c r="G10" s="31" t="n"/>
-      <c r="H10" s="31" t="n"/>
-      <c r="I10" s="31" t="n"/>
-      <c r="K10" s="31" t="n"/>
-      <c r="M10" s="31" t="n"/>
-      <c r="N10" s="33" t="n"/>
+      <c r="G10" s="31" t="inlineStr">
+        <is>
+          <t>3.5</t>
+        </is>
+      </c>
+      <c r="H10" s="31" t="inlineStr">
+        <is>
+          <t>4500</t>
+        </is>
+      </c>
+      <c r="I10" s="31" t="inlineStr">
+        <is>
+          <t>262.5</t>
+        </is>
+      </c>
+      <c r="K10" s="31" t="inlineStr">
+        <is>
+          <t>262.5</t>
+        </is>
+      </c>
+      <c r="M10" s="31" t="inlineStr">
+        <is>
+          <t>18025.0</t>
+        </is>
+      </c>
+      <c r="N10" s="32" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="30" t="n"/>
-      <c r="B11" s="31" t="n"/>
-      <c r="F11" s="31" t="n"/>
-      <c r="G11" s="31" t="n"/>
-      <c r="H11" s="31" t="n"/>
-      <c r="I11" s="31" t="n"/>
-      <c r="K11" s="31" t="n"/>
-      <c r="M11" s="31" t="n"/>
-      <c r="N11" s="33" t="n"/>
+      <c r="A11" s="33" t="n"/>
+      <c r="B11" s="34" t="n"/>
+      <c r="F11" s="34" t="n"/>
+      <c r="G11" s="34" t="n"/>
+      <c r="H11" s="34" t="n"/>
+      <c r="I11" s="34" t="n"/>
+      <c r="K11" s="34" t="n"/>
+      <c r="M11" s="34" t="n"/>
+      <c r="N11" s="32" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="30" t="n"/>
-      <c r="B12" s="31" t="n"/>
-      <c r="F12" s="31" t="n"/>
-      <c r="G12" s="31" t="n"/>
-      <c r="H12" s="31" t="n"/>
-      <c r="I12" s="31" t="n"/>
-      <c r="K12" s="31" t="n"/>
-      <c r="M12" s="31" t="n"/>
-      <c r="N12" s="33" t="n"/>
+      <c r="A12" s="33" t="n"/>
+      <c r="B12" s="34" t="n"/>
+      <c r="F12" s="34" t="n"/>
+      <c r="G12" s="34" t="n"/>
+      <c r="H12" s="34" t="n"/>
+      <c r="I12" s="34" t="n"/>
+      <c r="K12" s="34" t="n"/>
+      <c r="M12" s="34" t="n"/>
+      <c r="N12" s="32" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="30" t="n"/>
-      <c r="B13" s="31" t="n"/>
-      <c r="F13" s="31" t="n"/>
-      <c r="G13" s="31" t="n"/>
-      <c r="H13" s="31" t="n"/>
-      <c r="I13" s="31" t="n"/>
-      <c r="K13" s="31" t="n"/>
-      <c r="M13" s="31" t="n"/>
-      <c r="N13" s="33" t="n"/>
+      <c r="A13" s="33" t="n"/>
+      <c r="B13" s="34" t="n"/>
+      <c r="F13" s="34" t="n"/>
+      <c r="G13" s="34" t="n"/>
+      <c r="H13" s="34" t="n"/>
+      <c r="I13" s="34" t="n"/>
+      <c r="K13" s="34" t="n"/>
+      <c r="M13" s="34" t="n"/>
+      <c r="N13" s="32" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="30" t="n"/>
-      <c r="B14" s="31" t="n"/>
-      <c r="F14" s="31" t="n"/>
-      <c r="G14" s="31" t="n"/>
-      <c r="H14" s="31" t="n"/>
-      <c r="I14" s="31" t="n"/>
-      <c r="K14" s="31" t="n"/>
-      <c r="M14" s="31" t="n"/>
-      <c r="N14" s="33" t="n"/>
+      <c r="A14" s="33" t="n"/>
+      <c r="B14" s="34" t="n"/>
+      <c r="F14" s="34" t="n"/>
+      <c r="G14" s="34" t="n"/>
+      <c r="H14" s="34" t="n"/>
+      <c r="I14" s="34" t="n"/>
+      <c r="K14" s="34" t="n"/>
+      <c r="M14" s="34" t="n"/>
+      <c r="N14" s="32" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="30" t="n"/>
-      <c r="B15" s="31" t="n"/>
-      <c r="F15" s="31" t="n"/>
-      <c r="G15" s="31" t="n"/>
-      <c r="H15" s="31" t="n"/>
-      <c r="I15" s="31" t="n"/>
-      <c r="K15" s="31" t="n"/>
-      <c r="M15" s="31" t="n"/>
-      <c r="N15" s="33" t="n"/>
+      <c r="A15" s="33" t="n"/>
+      <c r="B15" s="34" t="n"/>
+      <c r="F15" s="34" t="n"/>
+      <c r="G15" s="34" t="n"/>
+      <c r="H15" s="34" t="n"/>
+      <c r="I15" s="34" t="n"/>
+      <c r="K15" s="34" t="n"/>
+      <c r="M15" s="34" t="n"/>
+      <c r="N15" s="32" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="30" t="n"/>
-      <c r="B16" s="31" t="n"/>
-      <c r="F16" s="31" t="n"/>
-      <c r="G16" s="31" t="n"/>
-      <c r="H16" s="31" t="n"/>
-      <c r="I16" s="31" t="n"/>
-      <c r="K16" s="31" t="n"/>
-      <c r="M16" s="31" t="n"/>
-      <c r="N16" s="33" t="n"/>
+      <c r="A16" s="33" t="n"/>
+      <c r="B16" s="34" t="n"/>
+      <c r="F16" s="34" t="n"/>
+      <c r="G16" s="34" t="n"/>
+      <c r="H16" s="34" t="n"/>
+      <c r="I16" s="34" t="n"/>
+      <c r="K16" s="34" t="n"/>
+      <c r="M16" s="34" t="n"/>
+      <c r="N16" s="32" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="30" t="n"/>
-      <c r="B17" s="31" t="n"/>
-      <c r="F17" s="31" t="n"/>
-      <c r="G17" s="31" t="n"/>
-      <c r="H17" s="31" t="n"/>
-      <c r="I17" s="31" t="n"/>
-      <c r="K17" s="31" t="n"/>
-      <c r="M17" s="31" t="n"/>
-      <c r="N17" s="33" t="n"/>
+      <c r="A17" s="33" t="n"/>
+      <c r="B17" s="34" t="n"/>
+      <c r="F17" s="34" t="n"/>
+      <c r="G17" s="34" t="n"/>
+      <c r="H17" s="34" t="n"/>
+      <c r="I17" s="34" t="n"/>
+      <c r="K17" s="34" t="n"/>
+      <c r="M17" s="34" t="n"/>
+      <c r="N17" s="32" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="34" t="n"/>
+      <c r="A18" s="35" t="n"/>
       <c r="B18" s="25" t="n"/>
       <c r="C18" s="26" t="n"/>
       <c r="D18" s="26" t="n"/>
       <c r="E18" s="27" t="n"/>
-      <c r="F18" s="35" t="n"/>
-      <c r="G18" s="35" t="n"/>
-      <c r="H18" s="35" t="n"/>
+      <c r="F18" s="36" t="n"/>
+      <c r="G18" s="36" t="n"/>
+      <c r="H18" s="36" t="n"/>
       <c r="I18" s="25" t="n"/>
       <c r="J18" s="27" t="n"/>
       <c r="K18" s="25" t="n"/>
@@ -1094,84 +1129,96 @@
       <c r="N18" s="18" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="36" t="n"/>
-      <c r="B19" s="37" t="n"/>
-      <c r="C19" s="38" t="n"/>
-      <c r="D19" s="39" t="inlineStr">
+      <c r="A19" s="37" t="n"/>
+      <c r="B19" s="38" t="n"/>
+      <c r="C19" s="39" t="n"/>
+      <c r="D19" s="40" t="inlineStr">
         <is>
           <t>Old Jewellery</t>
         </is>
       </c>
-      <c r="E19" s="38" t="n"/>
-      <c r="F19" s="38" t="n"/>
-      <c r="G19" s="40" t="n"/>
-      <c r="H19" s="37" t="n"/>
-      <c r="I19" s="41" t="inlineStr">
+      <c r="E19" s="39" t="n"/>
+      <c r="F19" s="39" t="n"/>
+      <c r="G19" s="41" t="n"/>
+      <c r="H19" s="38" t="n"/>
+      <c r="I19" s="42" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="J19" s="42" t="inlineStr">
+      <c r="J19" s="43" t="inlineStr">
         <is>
           <t>Unit Price</t>
         </is>
       </c>
-      <c r="K19" s="40" t="n"/>
-      <c r="L19" s="37" t="n"/>
-      <c r="M19" s="39" t="inlineStr">
+      <c r="K19" s="41" t="n"/>
+      <c r="L19" s="38" t="n"/>
+      <c r="M19" s="40" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="N19" s="43" t="n"/>
+      <c r="N19" s="44" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="44" t="n">
+      <c r="A20" s="45" t="n">
         <v>1</v>
       </c>
-      <c r="B20" s="45" t="inlineStr"/>
-      <c r="H20" s="31" t="n"/>
-      <c r="I20" s="45" t="inlineStr"/>
-      <c r="J20" s="32" t="inlineStr">
+      <c r="B20" s="46" t="inlineStr">
+        <is>
+          <t>old gold</t>
+        </is>
+      </c>
+      <c r="H20" s="34" t="n"/>
+      <c r="I20" s="46" t="inlineStr">
+        <is>
+          <t>3.5</t>
+        </is>
+      </c>
+      <c r="J20" s="31" t="inlineStr">
         <is>
           <t>4400</t>
         </is>
       </c>
-      <c r="L20" s="31" t="n"/>
-      <c r="M20" s="45" t="inlineStr"/>
-      <c r="N20" s="33" t="n"/>
+      <c r="L20" s="34" t="n"/>
+      <c r="M20" s="46" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="N20" s="32" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="46" t="n">
+      <c r="A21" s="47" t="n">
         <v>2</v>
       </c>
-      <c r="B21" s="45" t="inlineStr"/>
-      <c r="H21" s="31" t="n"/>
-      <c r="I21" s="45" t="inlineStr"/>
-      <c r="J21" s="32" t="inlineStr">
+      <c r="B21" s="46" t="inlineStr"/>
+      <c r="H21" s="34" t="n"/>
+      <c r="I21" s="46" t="inlineStr"/>
+      <c r="J21" s="31" t="inlineStr">
         <is>
           <t>4400</t>
         </is>
       </c>
-      <c r="L21" s="31" t="n"/>
-      <c r="M21" s="45" t="inlineStr"/>
-      <c r="N21" s="33" t="n"/>
+      <c r="L21" s="34" t="n"/>
+      <c r="M21" s="46" t="inlineStr"/>
+      <c r="N21" s="32" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="46" t="n">
+      <c r="A22" s="47" t="n">
         <v>3</v>
       </c>
-      <c r="B22" s="45" t="inlineStr"/>
-      <c r="H22" s="31" t="n"/>
-      <c r="I22" s="45" t="inlineStr"/>
-      <c r="J22" s="32" t="inlineStr">
+      <c r="B22" s="46" t="inlineStr"/>
+      <c r="H22" s="34" t="n"/>
+      <c r="I22" s="46" t="inlineStr"/>
+      <c r="J22" s="31" t="inlineStr">
         <is>
           <t>4400</t>
         </is>
       </c>
-      <c r="L22" s="31" t="n"/>
-      <c r="M22" s="45" t="inlineStr"/>
-      <c r="N22" s="33" t="n"/>
+      <c r="L22" s="34" t="n"/>
+      <c r="M22" s="46" t="inlineStr"/>
+      <c r="N22" s="32" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="15" t="n"/>
@@ -1190,160 +1237,160 @@
       <c r="N23" s="18" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="36" t="n"/>
-      <c r="B24" s="37" t="n"/>
-      <c r="C24" s="39" t="inlineStr">
+      <c r="A24" s="37" t="n"/>
+      <c r="B24" s="38" t="n"/>
+      <c r="C24" s="40" t="inlineStr">
         <is>
           <t>Other Addition Or Deduction</t>
         </is>
       </c>
-      <c r="D24" s="38" t="n"/>
-      <c r="E24" s="38" t="n"/>
-      <c r="F24" s="38" t="n"/>
-      <c r="G24" s="38" t="n"/>
-      <c r="H24" s="38" t="n"/>
-      <c r="I24" s="38" t="n"/>
-      <c r="J24" s="38" t="n"/>
-      <c r="K24" s="38" t="n"/>
-      <c r="L24" s="37" t="n"/>
-      <c r="M24" s="39" t="inlineStr">
+      <c r="D24" s="39" t="n"/>
+      <c r="E24" s="39" t="n"/>
+      <c r="F24" s="39" t="n"/>
+      <c r="G24" s="39" t="n"/>
+      <c r="H24" s="39" t="n"/>
+      <c r="I24" s="39" t="n"/>
+      <c r="J24" s="39" t="n"/>
+      <c r="K24" s="39" t="n"/>
+      <c r="L24" s="38" t="n"/>
+      <c r="M24" s="40" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="N24" s="43" t="n"/>
+      <c r="N24" s="44" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="47" t="n"/>
-      <c r="L25" s="48" t="n"/>
+      <c r="A25" s="48" t="n"/>
+      <c r="L25" s="49" t="n"/>
       <c r="N25" s="24" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="49" t="n"/>
-      <c r="L26" s="31" t="n"/>
-      <c r="N26" s="33" t="n"/>
+      <c r="A26" s="50" t="n"/>
+      <c r="L26" s="34" t="n"/>
+      <c r="N26" s="32" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="49" t="n"/>
+      <c r="A27" s="50" t="n"/>
       <c r="L27" s="25" t="n"/>
       <c r="N27" s="18" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="36" t="n"/>
-      <c r="B28" s="38" t="n"/>
-      <c r="C28" s="38" t="n"/>
-      <c r="D28" s="38" t="n"/>
-      <c r="E28" s="50" t="inlineStr">
+      <c r="A28" s="37" t="n"/>
+      <c r="B28" s="39" t="n"/>
+      <c r="C28" s="39" t="n"/>
+      <c r="D28" s="39" t="n"/>
+      <c r="E28" s="51" t="inlineStr">
         <is>
           <t>Mode Of Payment</t>
         </is>
       </c>
-      <c r="F28" s="38" t="n"/>
-      <c r="G28" s="38" t="n"/>
-      <c r="H28" s="38" t="n"/>
-      <c r="I28" s="51" t="inlineStr">
+      <c r="F28" s="39" t="n"/>
+      <c r="G28" s="39" t="n"/>
+      <c r="H28" s="39" t="n"/>
+      <c r="I28" s="52" t="inlineStr">
         <is>
           <t>Cash</t>
         </is>
       </c>
-      <c r="J28" s="38" t="n"/>
-      <c r="K28" s="38" t="n"/>
-      <c r="L28" s="38" t="n"/>
-      <c r="M28" s="38" t="n"/>
-      <c r="N28" s="43" t="n"/>
+      <c r="J28" s="39" t="n"/>
+      <c r="K28" s="39" t="n"/>
+      <c r="L28" s="39" t="n"/>
+      <c r="M28" s="39" t="n"/>
+      <c r="N28" s="44" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="52" t="inlineStr">
+      <c r="A29" s="53" t="inlineStr">
         <is>
           <t>Total in Words</t>
         </is>
       </c>
-      <c r="B29" s="38" t="n"/>
-      <c r="C29" s="51" t="inlineStr">
+      <c r="B29" s="39" t="n"/>
+      <c r="C29" s="52" t="inlineStr">
         <is>
           <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
         </is>
       </c>
-      <c r="D29" s="38" t="n"/>
-      <c r="E29" s="38" t="n"/>
-      <c r="F29" s="38" t="n"/>
-      <c r="G29" s="38" t="n"/>
-      <c r="H29" s="38" t="n"/>
-      <c r="I29" s="38" t="n"/>
-      <c r="J29" s="53" t="inlineStr">
+      <c r="D29" s="39" t="n"/>
+      <c r="E29" s="39" t="n"/>
+      <c r="F29" s="39" t="n"/>
+      <c r="G29" s="39" t="n"/>
+      <c r="H29" s="39" t="n"/>
+      <c r="I29" s="39" t="n"/>
+      <c r="J29" s="54" t="inlineStr">
         <is>
           <t xml:space="preserve">Total Paid : </t>
         </is>
       </c>
-      <c r="K29" s="38" t="n"/>
-      <c r="L29" s="51" t="inlineStr">
+      <c r="K29" s="39" t="n"/>
+      <c r="L29" s="52" t="inlineStr">
         <is>
           <t>2000000</t>
         </is>
       </c>
-      <c r="M29" s="38" t="n"/>
-      <c r="N29" s="43" t="n"/>
+      <c r="M29" s="39" t="n"/>
+      <c r="N29" s="44" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="54" t="n"/>
-      <c r="B30" s="55" t="inlineStr">
+      <c r="A30" s="55" t="n"/>
+      <c r="B30" s="56" t="inlineStr">
         <is>
           <t>Terms and conditions</t>
         </is>
       </c>
-      <c r="J30" s="48" t="n"/>
-      <c r="N30" s="33" t="n"/>
+      <c r="J30" s="49" t="n"/>
+      <c r="N30" s="32" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="56" t="inlineStr">
+      <c r="A31" s="57" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. Before taking delivery Customer should check the ornaments by piece and weight. </t>
         </is>
       </c>
-      <c r="J31" s="31" t="n"/>
-      <c r="N31" s="33" t="n"/>
+      <c r="J31" s="34" t="n"/>
+      <c r="N31" s="32" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="56" t="inlineStr">
+      <c r="A32" s="57" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2. Exchange your ornaments within 7 days in good condition.</t>
         </is>
       </c>
-      <c r="J32" s="31" t="n"/>
-      <c r="N32" s="33" t="n"/>
+      <c r="J32" s="34" t="n"/>
+      <c r="N32" s="32" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="56" t="inlineStr">
+      <c r="A33" s="57" t="inlineStr">
         <is>
           <t xml:space="preserve"> 3. We are not responsible for any damage or brakage after delivery</t>
         </is>
       </c>
-      <c r="J33" s="31" t="n"/>
-      <c r="N33" s="33" t="n"/>
+      <c r="J33" s="34" t="n"/>
+      <c r="N33" s="32" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="56" t="inlineStr">
+      <c r="A34" s="57" t="inlineStr">
         <is>
           <t xml:space="preserve"> 4. We can repair the ornaments if possible</t>
         </is>
       </c>
-      <c r="J34" s="31" t="n"/>
-      <c r="N34" s="57" t="n"/>
+      <c r="J34" s="34" t="n"/>
+      <c r="N34" s="58" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="58" t="n"/>
-      <c r="B35" s="58" t="n"/>
-      <c r="C35" s="58" t="n"/>
-      <c r="D35" s="58" t="n"/>
-      <c r="E35" s="58" t="n"/>
-      <c r="F35" s="58" t="n"/>
-      <c r="G35" s="58" t="n"/>
-      <c r="H35" s="58" t="n"/>
-      <c r="I35" s="58" t="n"/>
-      <c r="J35" s="58" t="n"/>
-      <c r="K35" s="58" t="n"/>
-      <c r="L35" s="58" t="n"/>
-      <c r="M35" s="58" t="n"/>
+      <c r="A35" s="59" t="n"/>
+      <c r="B35" s="59" t="n"/>
+      <c r="C35" s="59" t="n"/>
+      <c r="D35" s="59" t="n"/>
+      <c r="E35" s="59" t="n"/>
+      <c r="F35" s="59" t="n"/>
+      <c r="G35" s="59" t="n"/>
+      <c r="H35" s="59" t="n"/>
+      <c r="I35" s="59" t="n"/>
+      <c r="J35" s="59" t="n"/>
+      <c r="K35" s="59" t="n"/>
+      <c r="L35" s="59" t="n"/>
+      <c r="M35" s="59" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.2" top="0.2" bottom="0.2" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
printing paper size id reduced and some errors are removed and now we can store the location of the file and make new folder for every month
</commit_message>
<xml_diff>
--- a/FrontEnd/test.xlsx
+++ b/FrontEnd/test.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="bill" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -368,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -399,11 +399,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -414,12 +413,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -792,9 +788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -847,7 +843,11 @@
           <t xml:space="preserve">SI. No.: </t>
         </is>
       </c>
-      <c r="I5" s="8" t="inlineStr"/>
+      <c r="I5" s="8" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="J5" s="6" t="n"/>
       <c r="K5" s="7" t="inlineStr">
         <is>
@@ -864,11 +864,7 @@
           <t xml:space="preserve">Name: </t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr">
-        <is>
-          <t>ashu</t>
-        </is>
-      </c>
+      <c r="B6" s="11" t="inlineStr"/>
       <c r="F6" s="12" t="inlineStr">
         <is>
           <t>Mobile No.</t>
@@ -876,7 +872,7 @@
       </c>
       <c r="G6" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  7894100604</t>
+          <t xml:space="preserve">  </t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
@@ -884,17 +880,17 @@
           <t>Addhar No.</t>
         </is>
       </c>
-      <c r="J6" s="11" t="inlineStr">
-        <is>
-          <t>old town</t>
-        </is>
-      </c>
+      <c r="J6" s="11" t="inlineStr"/>
       <c r="M6" s="2" t="inlineStr">
         <is>
           <t>Bill No.</t>
         </is>
       </c>
-      <c r="N6" s="14" t="inlineStr"/>
+      <c r="N6" s="14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="15" t="n"/>
@@ -995,132 +991,106 @@
       <c r="N9" s="18" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="31" t="inlineStr">
-        <is>
-          <t>Ring</t>
-        </is>
-      </c>
-      <c r="F10" s="31" t="inlineStr">
+      <c r="A10" s="30" t="n"/>
+      <c r="B10" s="31" t="n"/>
+      <c r="F10" s="32" t="inlineStr">
         <is>
           <t>7113</t>
         </is>
       </c>
-      <c r="G10" s="31" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="H10" s="31" t="inlineStr">
-        <is>
-          <t>4500</t>
-        </is>
-      </c>
-      <c r="I10" s="31" t="inlineStr">
-        <is>
-          <t>262.5</t>
-        </is>
-      </c>
-      <c r="K10" s="31" t="inlineStr">
-        <is>
-          <t>262.5</t>
-        </is>
-      </c>
-      <c r="M10" s="31" t="inlineStr">
-        <is>
-          <t>18025.0</t>
-        </is>
-      </c>
-      <c r="N10" s="32" t="n"/>
+      <c r="G10" s="31" t="n"/>
+      <c r="H10" s="31" t="n"/>
+      <c r="I10" s="31" t="n"/>
+      <c r="K10" s="31" t="n"/>
+      <c r="M10" s="31" t="n"/>
+      <c r="N10" s="33" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="33" t="n"/>
-      <c r="B11" s="34" t="n"/>
-      <c r="F11" s="34" t="n"/>
-      <c r="G11" s="34" t="n"/>
-      <c r="H11" s="34" t="n"/>
-      <c r="I11" s="34" t="n"/>
-      <c r="K11" s="34" t="n"/>
-      <c r="M11" s="34" t="n"/>
-      <c r="N11" s="32" t="n"/>
+      <c r="A11" s="30" t="n"/>
+      <c r="B11" s="31" t="n"/>
+      <c r="F11" s="31" t="n"/>
+      <c r="G11" s="31" t="n"/>
+      <c r="H11" s="31" t="n"/>
+      <c r="I11" s="31" t="n"/>
+      <c r="K11" s="31" t="n"/>
+      <c r="M11" s="31" t="n"/>
+      <c r="N11" s="33" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="33" t="n"/>
-      <c r="B12" s="34" t="n"/>
-      <c r="F12" s="34" t="n"/>
-      <c r="G12" s="34" t="n"/>
-      <c r="H12" s="34" t="n"/>
-      <c r="I12" s="34" t="n"/>
-      <c r="K12" s="34" t="n"/>
-      <c r="M12" s="34" t="n"/>
-      <c r="N12" s="32" t="n"/>
+      <c r="A12" s="30" t="n"/>
+      <c r="B12" s="31" t="n"/>
+      <c r="F12" s="31" t="n"/>
+      <c r="G12" s="31" t="n"/>
+      <c r="H12" s="31" t="n"/>
+      <c r="I12" s="31" t="n"/>
+      <c r="K12" s="31" t="n"/>
+      <c r="M12" s="31" t="n"/>
+      <c r="N12" s="33" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="33" t="n"/>
-      <c r="B13" s="34" t="n"/>
-      <c r="F13" s="34" t="n"/>
-      <c r="G13" s="34" t="n"/>
-      <c r="H13" s="34" t="n"/>
-      <c r="I13" s="34" t="n"/>
-      <c r="K13" s="34" t="n"/>
-      <c r="M13" s="34" t="n"/>
-      <c r="N13" s="32" t="n"/>
+      <c r="A13" s="30" t="n"/>
+      <c r="B13" s="31" t="n"/>
+      <c r="F13" s="31" t="n"/>
+      <c r="G13" s="31" t="n"/>
+      <c r="H13" s="31" t="n"/>
+      <c r="I13" s="31" t="n"/>
+      <c r="K13" s="31" t="n"/>
+      <c r="M13" s="31" t="n"/>
+      <c r="N13" s="33" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="33" t="n"/>
-      <c r="B14" s="34" t="n"/>
-      <c r="F14" s="34" t="n"/>
-      <c r="G14" s="34" t="n"/>
-      <c r="H14" s="34" t="n"/>
-      <c r="I14" s="34" t="n"/>
-      <c r="K14" s="34" t="n"/>
-      <c r="M14" s="34" t="n"/>
-      <c r="N14" s="32" t="n"/>
+      <c r="A14" s="30" t="n"/>
+      <c r="B14" s="31" t="n"/>
+      <c r="F14" s="31" t="n"/>
+      <c r="G14" s="31" t="n"/>
+      <c r="H14" s="31" t="n"/>
+      <c r="I14" s="31" t="n"/>
+      <c r="K14" s="31" t="n"/>
+      <c r="M14" s="31" t="n"/>
+      <c r="N14" s="33" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="33" t="n"/>
-      <c r="B15" s="34" t="n"/>
-      <c r="F15" s="34" t="n"/>
-      <c r="G15" s="34" t="n"/>
-      <c r="H15" s="34" t="n"/>
-      <c r="I15" s="34" t="n"/>
-      <c r="K15" s="34" t="n"/>
-      <c r="M15" s="34" t="n"/>
-      <c r="N15" s="32" t="n"/>
+      <c r="A15" s="30" t="n"/>
+      <c r="B15" s="31" t="n"/>
+      <c r="F15" s="31" t="n"/>
+      <c r="G15" s="31" t="n"/>
+      <c r="H15" s="31" t="n"/>
+      <c r="I15" s="31" t="n"/>
+      <c r="K15" s="31" t="n"/>
+      <c r="M15" s="31" t="n"/>
+      <c r="N15" s="33" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="33" t="n"/>
-      <c r="B16" s="34" t="n"/>
-      <c r="F16" s="34" t="n"/>
-      <c r="G16" s="34" t="n"/>
-      <c r="H16" s="34" t="n"/>
-      <c r="I16" s="34" t="n"/>
-      <c r="K16" s="34" t="n"/>
-      <c r="M16" s="34" t="n"/>
-      <c r="N16" s="32" t="n"/>
+      <c r="A16" s="30" t="n"/>
+      <c r="B16" s="31" t="n"/>
+      <c r="F16" s="31" t="n"/>
+      <c r="G16" s="31" t="n"/>
+      <c r="H16" s="31" t="n"/>
+      <c r="I16" s="31" t="n"/>
+      <c r="K16" s="31" t="n"/>
+      <c r="M16" s="31" t="n"/>
+      <c r="N16" s="33" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="33" t="n"/>
-      <c r="B17" s="34" t="n"/>
-      <c r="F17" s="34" t="n"/>
-      <c r="G17" s="34" t="n"/>
-      <c r="H17" s="34" t="n"/>
-      <c r="I17" s="34" t="n"/>
-      <c r="K17" s="34" t="n"/>
-      <c r="M17" s="34" t="n"/>
-      <c r="N17" s="32" t="n"/>
+      <c r="A17" s="30" t="n"/>
+      <c r="B17" s="31" t="n"/>
+      <c r="F17" s="31" t="n"/>
+      <c r="G17" s="31" t="n"/>
+      <c r="H17" s="31" t="n"/>
+      <c r="I17" s="31" t="n"/>
+      <c r="K17" s="31" t="n"/>
+      <c r="M17" s="31" t="n"/>
+      <c r="N17" s="33" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="35" t="n"/>
+      <c r="A18" s="34" t="n"/>
       <c r="B18" s="25" t="n"/>
       <c r="C18" s="26" t="n"/>
       <c r="D18" s="26" t="n"/>
       <c r="E18" s="27" t="n"/>
-      <c r="F18" s="36" t="n"/>
-      <c r="G18" s="36" t="n"/>
-      <c r="H18" s="36" t="n"/>
+      <c r="F18" s="35" t="n"/>
+      <c r="G18" s="35" t="n"/>
+      <c r="H18" s="35" t="n"/>
       <c r="I18" s="25" t="n"/>
       <c r="J18" s="27" t="n"/>
       <c r="K18" s="25" t="n"/>
@@ -1129,96 +1099,57 @@
       <c r="N18" s="18" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="37" t="n"/>
-      <c r="B19" s="38" t="n"/>
-      <c r="C19" s="39" t="n"/>
-      <c r="D19" s="40" t="inlineStr">
+      <c r="A19" s="36" t="n"/>
+      <c r="B19" s="37" t="n"/>
+      <c r="C19" s="38" t="n"/>
+      <c r="D19" s="39" t="inlineStr">
         <is>
           <t>Old Jewellery</t>
         </is>
       </c>
-      <c r="E19" s="39" t="n"/>
-      <c r="F19" s="39" t="n"/>
-      <c r="G19" s="41" t="n"/>
-      <c r="H19" s="38" t="n"/>
-      <c r="I19" s="42" t="inlineStr">
+      <c r="E19" s="38" t="n"/>
+      <c r="F19" s="38" t="n"/>
+      <c r="G19" s="40" t="n"/>
+      <c r="H19" s="37" t="n"/>
+      <c r="I19" s="41" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="J19" s="43" t="inlineStr">
+      <c r="J19" s="42" t="inlineStr">
         <is>
           <t>Unit Price</t>
         </is>
       </c>
-      <c r="K19" s="41" t="n"/>
-      <c r="L19" s="38" t="n"/>
-      <c r="M19" s="40" t="inlineStr">
+      <c r="K19" s="40" t="n"/>
+      <c r="L19" s="37" t="n"/>
+      <c r="M19" s="39" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="N19" s="44" t="n"/>
+      <c r="N19" s="43" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="45" t="n">
-        <v>1</v>
-      </c>
-      <c r="B20" s="46" t="inlineStr">
-        <is>
-          <t>old gold</t>
-        </is>
-      </c>
-      <c r="H20" s="34" t="n"/>
-      <c r="I20" s="46" t="inlineStr">
-        <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="J20" s="31" t="inlineStr">
-        <is>
-          <t>4400</t>
-        </is>
-      </c>
-      <c r="L20" s="34" t="n"/>
-      <c r="M20" s="46" t="inlineStr">
-        <is>
-          <t>3000</t>
-        </is>
-      </c>
-      <c r="N20" s="32" t="n"/>
+      <c r="A20" s="44" t="n"/>
+      <c r="H20" s="31" t="n"/>
+      <c r="J20" s="31" t="n"/>
+      <c r="L20" s="31" t="n"/>
+      <c r="N20" s="33" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="47" t="n">
-        <v>2</v>
-      </c>
-      <c r="B21" s="46" t="inlineStr"/>
-      <c r="H21" s="34" t="n"/>
-      <c r="I21" s="46" t="inlineStr"/>
-      <c r="J21" s="31" t="inlineStr">
-        <is>
-          <t>4400</t>
-        </is>
-      </c>
-      <c r="L21" s="34" t="n"/>
-      <c r="M21" s="46" t="inlineStr"/>
-      <c r="N21" s="32" t="n"/>
+      <c r="A21" s="45" t="n"/>
+      <c r="H21" s="31" t="n"/>
+      <c r="J21" s="31" t="n"/>
+      <c r="L21" s="31" t="n"/>
+      <c r="N21" s="33" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="47" t="n">
-        <v>3</v>
-      </c>
-      <c r="B22" s="46" t="inlineStr"/>
-      <c r="H22" s="34" t="n"/>
-      <c r="I22" s="46" t="inlineStr"/>
-      <c r="J22" s="31" t="inlineStr">
-        <is>
-          <t>4400</t>
-        </is>
-      </c>
-      <c r="L22" s="34" t="n"/>
-      <c r="M22" s="46" t="inlineStr"/>
-      <c r="N22" s="32" t="n"/>
+      <c r="A22" s="45" t="n"/>
+      <c r="H22" s="31" t="n"/>
+      <c r="J22" s="31" t="n"/>
+      <c r="L22" s="31" t="n"/>
+      <c r="N22" s="33" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="15" t="n"/>
@@ -1237,163 +1168,150 @@
       <c r="N23" s="18" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="37" t="n"/>
-      <c r="B24" s="38" t="n"/>
-      <c r="C24" s="40" t="inlineStr">
+      <c r="A24" s="36" t="n"/>
+      <c r="B24" s="37" t="n"/>
+      <c r="C24" s="39" t="inlineStr">
         <is>
           <t>Other Addition Or Deduction</t>
         </is>
       </c>
-      <c r="D24" s="39" t="n"/>
-      <c r="E24" s="39" t="n"/>
-      <c r="F24" s="39" t="n"/>
-      <c r="G24" s="39" t="n"/>
-      <c r="H24" s="39" t="n"/>
-      <c r="I24" s="39" t="n"/>
-      <c r="J24" s="39" t="n"/>
-      <c r="K24" s="39" t="n"/>
-      <c r="L24" s="38" t="n"/>
-      <c r="M24" s="40" t="inlineStr">
+      <c r="D24" s="38" t="n"/>
+      <c r="E24" s="38" t="n"/>
+      <c r="F24" s="38" t="n"/>
+      <c r="G24" s="38" t="n"/>
+      <c r="H24" s="38" t="n"/>
+      <c r="I24" s="38" t="n"/>
+      <c r="J24" s="38" t="n"/>
+      <c r="K24" s="38" t="n"/>
+      <c r="L24" s="37" t="n"/>
+      <c r="M24" s="39" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="N24" s="44" t="n"/>
+      <c r="N24" s="43" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="48" t="n"/>
-      <c r="L25" s="49" t="n"/>
+      <c r="A25" s="44" t="n"/>
+      <c r="L25" s="46" t="n"/>
       <c r="N25" s="24" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="50" t="n"/>
-      <c r="L26" s="34" t="n"/>
-      <c r="N26" s="32" t="n"/>
+      <c r="A26" s="45" t="n"/>
+      <c r="L26" s="31" t="n"/>
+      <c r="N26" s="33" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="50" t="n"/>
+      <c r="A27" s="45" t="n"/>
       <c r="L27" s="25" t="n"/>
       <c r="N27" s="18" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="37" t="n"/>
-      <c r="B28" s="39" t="n"/>
-      <c r="C28" s="39" t="n"/>
-      <c r="D28" s="39" t="n"/>
-      <c r="E28" s="51" t="inlineStr">
+      <c r="A28" s="36" t="n"/>
+      <c r="B28" s="38" t="n"/>
+      <c r="C28" s="38" t="n"/>
+      <c r="D28" s="38" t="n"/>
+      <c r="E28" s="47" t="inlineStr">
         <is>
           <t>Mode Of Payment</t>
         </is>
       </c>
-      <c r="F28" s="39" t="n"/>
-      <c r="G28" s="39" t="n"/>
-      <c r="H28" s="39" t="n"/>
-      <c r="I28" s="52" t="inlineStr">
-        <is>
-          <t>Cash</t>
-        </is>
-      </c>
-      <c r="J28" s="39" t="n"/>
-      <c r="K28" s="39" t="n"/>
-      <c r="L28" s="39" t="n"/>
-      <c r="M28" s="39" t="n"/>
-      <c r="N28" s="44" t="n"/>
+      <c r="F28" s="38" t="n"/>
+      <c r="G28" s="38" t="n"/>
+      <c r="H28" s="38" t="n"/>
+      <c r="I28" s="48" t="inlineStr"/>
+      <c r="J28" s="38" t="n"/>
+      <c r="K28" s="38" t="n"/>
+      <c r="L28" s="38" t="n"/>
+      <c r="M28" s="38" t="n"/>
+      <c r="N28" s="43" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="53" t="inlineStr">
+      <c r="A29" s="49" t="inlineStr">
         <is>
           <t>Total in Words</t>
         </is>
       </c>
-      <c r="B29" s="39" t="n"/>
-      <c r="C29" s="52" t="inlineStr">
+      <c r="B29" s="38" t="n"/>
+      <c r="C29" s="48" t="inlineStr">
         <is>
           <t>aaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaaa</t>
         </is>
       </c>
-      <c r="D29" s="39" t="n"/>
-      <c r="E29" s="39" t="n"/>
-      <c r="F29" s="39" t="n"/>
-      <c r="G29" s="39" t="n"/>
-      <c r="H29" s="39" t="n"/>
-      <c r="I29" s="39" t="n"/>
-      <c r="J29" s="54" t="inlineStr">
+      <c r="D29" s="38" t="n"/>
+      <c r="E29" s="38" t="n"/>
+      <c r="F29" s="38" t="n"/>
+      <c r="G29" s="38" t="n"/>
+      <c r="H29" s="38" t="n"/>
+      <c r="I29" s="38" t="n"/>
+      <c r="J29" s="50" t="inlineStr">
         <is>
           <t xml:space="preserve">Total Paid : </t>
         </is>
       </c>
-      <c r="K29" s="39" t="n"/>
-      <c r="L29" s="52" t="inlineStr">
-        <is>
-          <t>2000000</t>
-        </is>
-      </c>
-      <c r="M29" s="39" t="n"/>
-      <c r="N29" s="44" t="n"/>
+      <c r="K29" s="38" t="n"/>
+      <c r="L29" s="48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M29" s="38" t="n"/>
+      <c r="N29" s="43" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="55" t="n"/>
-      <c r="B30" s="56" t="inlineStr">
+      <c r="A30" s="51" t="n"/>
+      <c r="B30" s="52" t="inlineStr">
         <is>
           <t>Terms and conditions</t>
         </is>
       </c>
-      <c r="J30" s="49" t="n"/>
-      <c r="N30" s="32" t="n"/>
+      <c r="J30" s="46" t="n"/>
+      <c r="N30" s="33" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="57" t="inlineStr">
+      <c r="A31" s="53" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. Before taking delivery Customer should check the ornaments by piece and weight. </t>
         </is>
       </c>
-      <c r="J31" s="34" t="n"/>
-      <c r="N31" s="32" t="n"/>
+      <c r="J31" s="31" t="n"/>
+      <c r="N31" s="33" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="57" t="inlineStr">
+      <c r="A32" s="53" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2. Exchange your ornaments within 7 days in good condition.</t>
         </is>
       </c>
-      <c r="J32" s="34" t="n"/>
-      <c r="N32" s="32" t="n"/>
+      <c r="J32" s="31" t="n"/>
+      <c r="N32" s="33" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="57" t="inlineStr">
+      <c r="A33" s="53" t="inlineStr">
         <is>
           <t xml:space="preserve"> 3. We are not responsible for any damage or brakage after delivery</t>
         </is>
       </c>
-      <c r="J33" s="34" t="n"/>
-      <c r="N33" s="32" t="n"/>
+      <c r="J33" s="31" t="n"/>
+      <c r="N33" s="54" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="57" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 4. We can repair the ornaments if possible</t>
-        </is>
-      </c>
-      <c r="J34" s="34" t="n"/>
-      <c r="N34" s="58" t="n"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="59" t="n"/>
-      <c r="B35" s="59" t="n"/>
-      <c r="C35" s="59" t="n"/>
-      <c r="D35" s="59" t="n"/>
-      <c r="E35" s="59" t="n"/>
-      <c r="F35" s="59" t="n"/>
-      <c r="G35" s="59" t="n"/>
-      <c r="H35" s="59" t="n"/>
-      <c r="I35" s="59" t="n"/>
-      <c r="J35" s="59" t="n"/>
-      <c r="K35" s="59" t="n"/>
-      <c r="L35" s="59" t="n"/>
-      <c r="M35" s="59" t="n"/>
+      <c r="A34" s="55" t="n"/>
+      <c r="B34" s="55" t="n"/>
+      <c r="C34" s="55" t="n"/>
+      <c r="D34" s="55" t="n"/>
+      <c r="E34" s="55" t="n"/>
+      <c r="F34" s="55" t="n"/>
+      <c r="G34" s="55" t="n"/>
+      <c r="H34" s="55" t="n"/>
+      <c r="I34" s="55" t="n"/>
+      <c r="J34" s="55" t="n"/>
+      <c r="K34" s="55" t="n"/>
+      <c r="L34" s="55" t="n"/>
+      <c r="M34" s="55" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.2" top="0.2" bottom="0.2" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" paperSize="2"/>
+  <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup orientation="landscape" paperSize="13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added arrow gst content gold rate and find partially
</commit_message>
<xml_diff>
--- a/FrontEnd/test.xlsx
+++ b/FrontEnd/test.xlsx
@@ -373,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -406,11 +406,13 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="13" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -852,12 +854,12 @@
         </is>
       </c>
       <c r="I5" s="8" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="J5" s="6" t="n"/>
       <c r="K5" s="7" t="inlineStr">
         <is>
-          <t>Date: 07-Mar-22 - (Monday)</t>
+          <t>Date: 12-Mar-22 - (Saturday)</t>
         </is>
       </c>
       <c r="L5" s="6" t="n"/>
@@ -870,7 +872,11 @@
           <t xml:space="preserve">Name: </t>
         </is>
       </c>
-      <c r="B6" s="11" t="inlineStr"/>
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>ashu</t>
+        </is>
+      </c>
       <c r="F6" s="12" t="inlineStr">
         <is>
           <t>Mobile No.</t>
@@ -878,7 +884,7 @@
       </c>
       <c r="G6" s="13" t="inlineStr">
         <is>
-          <t xml:space="preserve">  </t>
+          <t xml:space="preserve">  7894100604</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
@@ -886,14 +892,18 @@
           <t>Addhar No.</t>
         </is>
       </c>
-      <c r="J6" s="11" t="inlineStr"/>
+      <c r="J6" s="11" t="inlineStr">
+        <is>
+          <t>11212</t>
+        </is>
+      </c>
       <c r="M6" s="2" t="inlineStr">
         <is>
           <t>Bill No.</t>
         </is>
       </c>
       <c r="N6" s="14" t="n">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
@@ -999,115 +1009,151 @@
       <c r="N9" s="18" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="32" t="n"/>
-      <c r="B10" s="33" t="n"/>
+      <c r="A10" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="33" t="inlineStr">
+        <is>
+          <t>Ring</t>
+        </is>
+      </c>
       <c r="D10" s="22" t="n"/>
       <c r="E10" s="34" t="inlineStr">
         <is>
           <t>7113</t>
         </is>
       </c>
-      <c r="F10" s="33" t="n"/>
-      <c r="G10" s="33" t="n"/>
-      <c r="H10" s="33" t="n"/>
-      <c r="I10" s="33" t="n"/>
-      <c r="K10" s="33" t="n"/>
-      <c r="M10" s="33" t="n"/>
+      <c r="F10" s="33" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="G10" s="33" t="n">
+        <v>629.17</v>
+      </c>
+      <c r="H10" s="33" t="n">
+        <v>4876</v>
+      </c>
+      <c r="I10" s="33" t="n">
+        <v>375.73</v>
+      </c>
+      <c r="K10" s="33" t="n">
+        <v>375.73</v>
+      </c>
+      <c r="M10" s="33" t="n">
+        <v>25800</v>
+      </c>
       <c r="N10" s="35" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="32" t="n"/>
-      <c r="B11" s="33" t="n"/>
+      <c r="A11" s="32" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" s="33" t="inlineStr">
+        <is>
+          <t>Ring</t>
+        </is>
+      </c>
       <c r="D11" s="36" t="n"/>
-      <c r="F11" s="33" t="n"/>
-      <c r="G11" s="33" t="n"/>
-      <c r="H11" s="33" t="n"/>
-      <c r="I11" s="33" t="n"/>
-      <c r="K11" s="33" t="n"/>
-      <c r="M11" s="33" t="n"/>
+      <c r="F11" s="33" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G11" s="33" t="n">
+        <v>394.46</v>
+      </c>
+      <c r="H11" s="33" t="n">
+        <v>4876</v>
+      </c>
+      <c r="I11" s="33" t="n">
+        <v>276.7</v>
+      </c>
+      <c r="K11" s="33" t="n">
+        <v>276.7</v>
+      </c>
+      <c r="M11" s="33" t="n">
+        <v>19000</v>
+      </c>
       <c r="N11" s="35" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="32" t="n"/>
-      <c r="B12" s="33" t="n"/>
+      <c r="A12" s="37" t="n"/>
+      <c r="B12" s="38" t="n"/>
       <c r="D12" s="36" t="n"/>
-      <c r="F12" s="33" t="n"/>
-      <c r="G12" s="33" t="n"/>
-      <c r="H12" s="33" t="n"/>
-      <c r="I12" s="33" t="n"/>
-      <c r="K12" s="33" t="n"/>
-      <c r="M12" s="33" t="n"/>
+      <c r="F12" s="38" t="n"/>
+      <c r="G12" s="38" t="n"/>
+      <c r="H12" s="38" t="n"/>
+      <c r="I12" s="38" t="n"/>
+      <c r="K12" s="38" t="n"/>
+      <c r="M12" s="38" t="n"/>
       <c r="N12" s="35" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="32" t="n"/>
-      <c r="B13" s="33" t="n"/>
+      <c r="A13" s="37" t="n"/>
+      <c r="B13" s="38" t="n"/>
       <c r="D13" s="36" t="n"/>
-      <c r="F13" s="33" t="n"/>
-      <c r="G13" s="33" t="n"/>
-      <c r="H13" s="33" t="n"/>
-      <c r="I13" s="33" t="n"/>
-      <c r="K13" s="33" t="n"/>
-      <c r="M13" s="33" t="n"/>
+      <c r="F13" s="38" t="n"/>
+      <c r="G13" s="38" t="n"/>
+      <c r="H13" s="38" t="n"/>
+      <c r="I13" s="38" t="n"/>
+      <c r="K13" s="38" t="n"/>
+      <c r="M13" s="38" t="n"/>
       <c r="N13" s="35" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="32" t="n"/>
-      <c r="B14" s="33" t="n"/>
+      <c r="A14" s="37" t="n"/>
+      <c r="B14" s="38" t="n"/>
       <c r="D14" s="36" t="n"/>
-      <c r="F14" s="33" t="n"/>
-      <c r="G14" s="33" t="n"/>
-      <c r="H14" s="33" t="n"/>
-      <c r="I14" s="33" t="n"/>
-      <c r="K14" s="33" t="n"/>
-      <c r="M14" s="33" t="n"/>
+      <c r="F14" s="38" t="n"/>
+      <c r="G14" s="38" t="n"/>
+      <c r="H14" s="38" t="n"/>
+      <c r="I14" s="38" t="n"/>
+      <c r="K14" s="38" t="n"/>
+      <c r="M14" s="38" t="n"/>
       <c r="N14" s="35" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="32" t="n"/>
-      <c r="B15" s="33" t="n"/>
+      <c r="A15" s="37" t="n"/>
+      <c r="B15" s="38" t="n"/>
       <c r="D15" s="36" t="n"/>
-      <c r="F15" s="33" t="n"/>
-      <c r="G15" s="33" t="n"/>
-      <c r="H15" s="33" t="n"/>
-      <c r="I15" s="33" t="n"/>
-      <c r="K15" s="33" t="n"/>
-      <c r="M15" s="33" t="n"/>
+      <c r="F15" s="38" t="n"/>
+      <c r="G15" s="38" t="n"/>
+      <c r="H15" s="38" t="n"/>
+      <c r="I15" s="38" t="n"/>
+      <c r="K15" s="38" t="n"/>
+      <c r="M15" s="38" t="n"/>
       <c r="N15" s="35" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="32" t="n"/>
-      <c r="B16" s="33" t="n"/>
+      <c r="A16" s="37" t="n"/>
+      <c r="B16" s="38" t="n"/>
       <c r="D16" s="36" t="n"/>
-      <c r="F16" s="33" t="n"/>
-      <c r="G16" s="33" t="n"/>
-      <c r="H16" s="33" t="n"/>
-      <c r="I16" s="33" t="n"/>
-      <c r="K16" s="33" t="n"/>
-      <c r="M16" s="33" t="n"/>
+      <c r="F16" s="38" t="n"/>
+      <c r="G16" s="38" t="n"/>
+      <c r="H16" s="38" t="n"/>
+      <c r="I16" s="38" t="n"/>
+      <c r="K16" s="38" t="n"/>
+      <c r="M16" s="38" t="n"/>
       <c r="N16" s="35" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="32" t="n"/>
-      <c r="B17" s="33" t="n"/>
+      <c r="A17" s="37" t="n"/>
+      <c r="B17" s="38" t="n"/>
       <c r="D17" s="36" t="n"/>
-      <c r="F17" s="33" t="n"/>
-      <c r="G17" s="33" t="n"/>
-      <c r="H17" s="33" t="n"/>
-      <c r="I17" s="33" t="n"/>
-      <c r="K17" s="33" t="n"/>
-      <c r="M17" s="33" t="n"/>
+      <c r="F17" s="38" t="n"/>
+      <c r="G17" s="38" t="n"/>
+      <c r="H17" s="38" t="n"/>
+      <c r="I17" s="38" t="n"/>
+      <c r="K17" s="38" t="n"/>
+      <c r="M17" s="38" t="n"/>
       <c r="N17" s="35" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="37" t="n"/>
+      <c r="A18" s="39" t="n"/>
       <c r="B18" s="26" t="n"/>
       <c r="C18" s="27" t="n"/>
       <c r="D18" s="28" t="n"/>
       <c r="E18" s="28" t="n"/>
-      <c r="F18" s="38" t="n"/>
-      <c r="G18" s="38" t="n"/>
-      <c r="H18" s="38" t="n"/>
+      <c r="F18" s="40" t="n"/>
+      <c r="G18" s="40" t="n"/>
+      <c r="H18" s="40" t="n"/>
       <c r="I18" s="26" t="n"/>
       <c r="J18" s="28" t="n"/>
       <c r="K18" s="26" t="n"/>
@@ -1116,56 +1162,56 @@
       <c r="N18" s="18" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="39" t="n"/>
-      <c r="B19" s="40" t="n"/>
-      <c r="C19" s="41" t="n"/>
-      <c r="D19" s="42" t="inlineStr">
+      <c r="A19" s="41" t="n"/>
+      <c r="B19" s="42" t="n"/>
+      <c r="C19" s="43" t="n"/>
+      <c r="D19" s="44" t="inlineStr">
         <is>
           <t>Old Jewellery</t>
         </is>
       </c>
-      <c r="E19" s="41" t="n"/>
-      <c r="F19" s="41" t="n"/>
-      <c r="G19" s="43" t="n"/>
-      <c r="H19" s="40" t="n"/>
-      <c r="I19" s="44" t="inlineStr">
+      <c r="E19" s="43" t="n"/>
+      <c r="F19" s="43" t="n"/>
+      <c r="G19" s="45" t="n"/>
+      <c r="H19" s="42" t="n"/>
+      <c r="I19" s="46" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="J19" s="45" t="inlineStr">
+      <c r="J19" s="47" t="inlineStr">
         <is>
           <t>Unit Price</t>
         </is>
       </c>
-      <c r="K19" s="43" t="n"/>
-      <c r="L19" s="40" t="n"/>
-      <c r="M19" s="42" t="inlineStr">
+      <c r="K19" s="45" t="n"/>
+      <c r="L19" s="42" t="n"/>
+      <c r="M19" s="44" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="N19" s="46" t="n"/>
+      <c r="N19" s="48" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="47" t="n"/>
-      <c r="H20" s="33" t="n"/>
-      <c r="J20" s="33" t="n"/>
-      <c r="L20" s="33" t="n"/>
+      <c r="A20" s="49" t="n"/>
+      <c r="H20" s="38" t="n"/>
+      <c r="J20" s="38" t="n"/>
+      <c r="L20" s="38" t="n"/>
       <c r="N20" s="35" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="48" t="n"/>
-      <c r="H21" s="33" t="n"/>
-      <c r="J21" s="33" t="n"/>
-      <c r="L21" s="33" t="n"/>
+      <c r="A21" s="50" t="n"/>
+      <c r="H21" s="38" t="n"/>
+      <c r="J21" s="38" t="n"/>
+      <c r="L21" s="38" t="n"/>
       <c r="N21" s="35" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="48" t="n"/>
-      <c r="H22" s="33" t="n"/>
-      <c r="J22" s="33" t="n"/>
-      <c r="L22" s="33" t="n"/>
+      <c r="A22" s="50" t="n"/>
+      <c r="H22" s="38" t="n"/>
+      <c r="J22" s="38" t="n"/>
+      <c r="L22" s="38" t="n"/>
       <c r="N22" s="35" t="n"/>
     </row>
     <row r="23">
@@ -1185,143 +1231,147 @@
       <c r="N23" s="18" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="39" t="n"/>
-      <c r="B24" s="40" t="n"/>
-      <c r="C24" s="42" t="inlineStr">
+      <c r="A24" s="41" t="n"/>
+      <c r="B24" s="42" t="n"/>
+      <c r="C24" s="44" t="inlineStr">
         <is>
           <t>Other Addition Or Deduction</t>
         </is>
       </c>
-      <c r="D24" s="41" t="n"/>
-      <c r="E24" s="41" t="n"/>
-      <c r="F24" s="41" t="n"/>
-      <c r="G24" s="41" t="n"/>
-      <c r="H24" s="41" t="n"/>
-      <c r="I24" s="41" t="n"/>
-      <c r="J24" s="41" t="n"/>
-      <c r="K24" s="41" t="n"/>
-      <c r="L24" s="40" t="n"/>
-      <c r="M24" s="42" t="inlineStr">
+      <c r="D24" s="43" t="n"/>
+      <c r="E24" s="43" t="n"/>
+      <c r="F24" s="43" t="n"/>
+      <c r="G24" s="43" t="n"/>
+      <c r="H24" s="43" t="n"/>
+      <c r="I24" s="43" t="n"/>
+      <c r="J24" s="43" t="n"/>
+      <c r="K24" s="43" t="n"/>
+      <c r="L24" s="42" t="n"/>
+      <c r="M24" s="44" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="N24" s="46" t="n"/>
+      <c r="N24" s="48" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="47" t="n"/>
-      <c r="L25" s="49" t="n"/>
+      <c r="A25" s="49" t="n"/>
+      <c r="L25" s="51" t="n"/>
       <c r="N25" s="25" t="n"/>
     </row>
     <row r="26">
-      <c r="A26" s="48" t="n"/>
-      <c r="L26" s="33" t="n"/>
+      <c r="A26" s="50" t="n"/>
+      <c r="L26" s="38" t="n"/>
       <c r="N26" s="35" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="48" t="n"/>
+      <c r="A27" s="50" t="n"/>
       <c r="L27" s="26" t="n"/>
       <c r="N27" s="18" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="39" t="n"/>
-      <c r="B28" s="41" t="n"/>
-      <c r="C28" s="41" t="n"/>
-      <c r="D28" s="41" t="n"/>
-      <c r="E28" s="50" t="inlineStr">
+      <c r="A28" s="41" t="n"/>
+      <c r="B28" s="43" t="n"/>
+      <c r="C28" s="43" t="n"/>
+      <c r="D28" s="43" t="n"/>
+      <c r="E28" s="52" t="inlineStr">
         <is>
           <t>Mode Of Payment</t>
         </is>
       </c>
-      <c r="F28" s="41" t="n"/>
-      <c r="G28" s="41" t="n"/>
-      <c r="H28" s="41" t="n"/>
-      <c r="I28" s="51" t="inlineStr"/>
-      <c r="J28" s="41" t="n"/>
-      <c r="K28" s="41" t="n"/>
-      <c r="L28" s="41" t="n"/>
-      <c r="M28" s="41" t="n"/>
-      <c r="N28" s="46" t="n"/>
+      <c r="F28" s="43" t="n"/>
+      <c r="G28" s="43" t="n"/>
+      <c r="H28" s="43" t="n"/>
+      <c r="I28" s="53" t="inlineStr"/>
+      <c r="J28" s="43" t="n"/>
+      <c r="K28" s="43" t="n"/>
+      <c r="L28" s="43" t="n"/>
+      <c r="M28" s="43" t="n"/>
+      <c r="N28" s="48" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="52" t="inlineStr">
+      <c r="A29" s="54" t="inlineStr">
         <is>
           <t>Total in Words</t>
         </is>
       </c>
-      <c r="B29" s="41" t="n"/>
-      <c r="C29" s="51" t="inlineStr"/>
-      <c r="D29" s="41" t="n"/>
-      <c r="E29" s="41" t="n"/>
-      <c r="F29" s="41" t="n"/>
-      <c r="G29" s="41" t="n"/>
-      <c r="H29" s="41" t="n"/>
-      <c r="I29" s="41" t="n"/>
-      <c r="J29" s="53" t="inlineStr">
+      <c r="B29" s="43" t="n"/>
+      <c r="C29" s="53" t="inlineStr">
+        <is>
+          <t>Forty Four Thousand, Eight Hundred</t>
+        </is>
+      </c>
+      <c r="D29" s="43" t="n"/>
+      <c r="E29" s="43" t="n"/>
+      <c r="F29" s="43" t="n"/>
+      <c r="G29" s="43" t="n"/>
+      <c r="H29" s="43" t="n"/>
+      <c r="I29" s="43" t="n"/>
+      <c r="J29" s="55" t="inlineStr">
         <is>
           <t xml:space="preserve">Total Paid : </t>
         </is>
       </c>
-      <c r="K29" s="41" t="n"/>
-      <c r="L29" s="51" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M29" s="41" t="n"/>
-      <c r="N29" s="46" t="n"/>
+      <c r="K29" s="43" t="n"/>
+      <c r="L29" s="53" t="inlineStr">
+        <is>
+          <t>44800</t>
+        </is>
+      </c>
+      <c r="M29" s="43" t="n"/>
+      <c r="N29" s="48" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="54" t="n"/>
-      <c r="B30" s="55" t="inlineStr">
+      <c r="A30" s="56" t="n"/>
+      <c r="B30" s="57" t="inlineStr">
         <is>
           <t>Terms and conditions</t>
         </is>
       </c>
-      <c r="J30" s="49" t="n"/>
+      <c r="J30" s="51" t="n"/>
       <c r="N30" s="35" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="56" t="inlineStr">
+      <c r="A31" s="58" t="inlineStr">
         <is>
           <t xml:space="preserve"> 1. Before taking delivery Customer should check the ornaments by piece and weight. </t>
         </is>
       </c>
-      <c r="J31" s="33" t="n"/>
+      <c r="J31" s="38" t="n"/>
       <c r="N31" s="35" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="56" t="inlineStr">
+      <c r="A32" s="58" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2. Exchange your ornaments within 7 days in good condition.</t>
         </is>
       </c>
-      <c r="J32" s="33" t="n"/>
+      <c r="J32" s="38" t="n"/>
       <c r="N32" s="35" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="56" t="inlineStr">
+      <c r="A33" s="58" t="inlineStr">
         <is>
           <t xml:space="preserve"> 3. We are not responsible for any damage or brakage after delivery</t>
         </is>
       </c>
-      <c r="J33" s="33" t="n"/>
-      <c r="N33" s="57" t="n"/>
+      <c r="J33" s="38" t="n"/>
+      <c r="N33" s="59" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="58" t="n"/>
-      <c r="B34" s="58" t="n"/>
-      <c r="C34" s="58" t="n"/>
-      <c r="D34" s="58" t="n"/>
-      <c r="E34" s="58" t="n"/>
-      <c r="F34" s="58" t="n"/>
-      <c r="G34" s="58" t="n"/>
-      <c r="H34" s="58" t="n"/>
-      <c r="I34" s="58" t="n"/>
-      <c r="J34" s="58" t="n"/>
-      <c r="K34" s="58" t="n"/>
-      <c r="L34" s="58" t="n"/>
-      <c r="M34" s="58" t="n"/>
+      <c r="A34" s="60" t="n"/>
+      <c r="B34" s="60" t="n"/>
+      <c r="C34" s="60" t="n"/>
+      <c r="D34" s="60" t="n"/>
+      <c r="E34" s="60" t="n"/>
+      <c r="F34" s="60" t="n"/>
+      <c r="G34" s="60" t="n"/>
+      <c r="H34" s="60" t="n"/>
+      <c r="I34" s="60" t="n"/>
+      <c r="J34" s="60" t="n"/>
+      <c r="K34" s="60" t="n"/>
+      <c r="L34" s="60" t="n"/>
+      <c r="M34" s="60" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>